<commit_message>
IEN-855 save 'registration destination' to notes
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC134596-49BB-D648-922F-186B1DE7B65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD863759-8C45-6B4B-B6F1-992BE4358E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-780" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="542">
   <si>
     <t>Last Name</t>
   </si>
@@ -2250,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2341,6 +2341,9 @@
       <c r="M2" s="9">
         <v>44562</v>
       </c>
+      <c r="P2" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3">
@@ -2361,6 +2364,9 @@
       <c r="M3" s="9">
         <v>44593</v>
       </c>
+      <c r="P3" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4">
@@ -2378,6 +2384,9 @@
       <c r="I4" t="s">
         <v>532</v>
       </c>
+      <c r="P4" s="11" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
@@ -2394,6 +2403,9 @@
       </c>
       <c r="I5" t="s">
         <v>527</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16">

</xml_diff>

<commit_message>
IEN-855 Add BCCNM/NCAS role (#579)
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC134596-49BB-D648-922F-186B1DE7B65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD863759-8C45-6B4B-B6F1-992BE4358E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-780" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="542">
   <si>
     <t>Last Name</t>
   </si>
@@ -2250,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2341,6 +2341,9 @@
       <c r="M2" s="9">
         <v>44562</v>
       </c>
+      <c r="P2" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3">
@@ -2361,6 +2364,9 @@
       <c r="M3" s="9">
         <v>44593</v>
       </c>
+      <c r="P3" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4">
@@ -2378,6 +2384,9 @@
       <c r="I4" t="s">
         <v>532</v>
       </c>
+      <c r="P4" s="11" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
@@ -2394,6 +2403,9 @@
       </c>
       <c r="I5" t="s">
         <v>527</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16">

</xml_diff>

<commit_message>
IEN-870 create 'applied to bccnm' and 'complete ncas' milestone from spreadsheet
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD863759-8C45-6B4B-B6F1-992BE4358E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63930764-07AB-D44A-B008-1911F4D6EFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-780" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="542">
   <si>
     <t>Last Name</t>
   </si>
@@ -79,12 +79,6 @@
     <t>Zip/Postal Code</t>
   </si>
   <si>
-    <t>NCAS Asssessment Complete</t>
-  </si>
-  <si>
-    <t>BCCN Application Complete</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yes </t>
   </si>
   <si>
@@ -1664,6 +1658,12 @@
   </si>
   <si>
     <t>Robert.Frederick_648@acme.com</t>
+  </si>
+  <si>
+    <t>BCCNM Application Complete</t>
+  </si>
+  <si>
+    <t>NCAS Assessment Complete</t>
   </si>
 </sst>
 </file>
@@ -1943,8 +1943,8 @@
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[Country of Education]],Sheet1!C2:D250,2,0),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{A3485428-BB17-4719-9693-9A5D42422885}" name="Date ROS Contract Signed" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{C528BBBE-AF13-4DE4-8CB9-6A5D36322874}" name="NCAS Asssessment Complete" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{FC5EB113-2259-4AAD-B918-D66D8CDC1B70}" name="BCCN Application Complete" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{C528BBBE-AF13-4DE4-8CB9-6A5D36322874}" name="NCAS Assessment Complete" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{FC5EB113-2259-4AAD-B918-D66D8CDC1B70}" name="BCCNM Application Complete" dataDxfId="1"/>
     <tableColumn id="15" xr3:uid="{2EEE535B-18BF-4006-8377-F5D12DDCB956}" name="Registration Designation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2250,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2277,7 +2277,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -2304,22 +2304,22 @@
         <v>12</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>13</v>
+        <v>541</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>14</v>
+        <v>540</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -2327,22 +2327,28 @@
         <v>112374</v>
       </c>
       <c r="C2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>536</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>538</v>
-      </c>
       <c r="I2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="M2" s="9">
         <v>44562</v>
       </c>
+      <c r="N2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="P2" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2350,22 +2356,28 @@
         <v>111166</v>
       </c>
       <c r="C3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D3" t="s">
+        <v>531</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>533</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>535</v>
-      </c>
       <c r="I3" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="M3" s="9">
         <v>44593</v>
       </c>
+      <c r="N3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="P3" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -2373,19 +2385,19 @@
         <v>111208</v>
       </c>
       <c r="C4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D4" t="s">
+        <v>537</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>539</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>541</v>
-      </c>
       <c r="I4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2393,19 +2405,19 @@
         <v>999999</v>
       </c>
       <c r="C5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D5" t="s">
+        <v>526</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>528</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>530</v>
-      </c>
       <c r="I5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -3042,7 +3054,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:O3 N4 N5:O59</xm:sqref>
+          <xm:sqref>N5:O59 O2:O3 N2:N4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41C196C3-3B03-4A85-A4EF-7D46FACB4C5B}">
           <x14:formula1>
@@ -3092,7 +3104,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -3175,2032 +3187,2032 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="C8" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="C10" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="C11" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="C12" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="C13" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="C14" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="C15" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="C16" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="3:4">
       <c r="C19" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="3:4">
       <c r="C20" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="3:4">
       <c r="C21" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="3:4">
       <c r="C22" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="3:4">
       <c r="C24" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="3:4">
       <c r="C25" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="3:4">
       <c r="C26" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="3:4">
       <c r="C27" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="3:4">
       <c r="C28" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="3:4">
       <c r="C29" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="3:4">
       <c r="C30" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="3:4">
       <c r="C31" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="3:4">
       <c r="C32" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="3:4">
       <c r="C81" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="3:4">
       <c r="C82" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="3:4">
       <c r="C83" s="13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="84" spans="3:4">
       <c r="C84" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="3:4">
       <c r="C85" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="86" spans="3:4">
       <c r="C86" s="13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="3:4">
       <c r="C87" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="88" spans="3:4">
       <c r="C88" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="89" spans="3:4">
       <c r="C89" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" spans="3:4">
       <c r="C90" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="91" spans="3:4">
       <c r="C91" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" spans="3:4">
       <c r="C92" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="93" spans="3:4">
       <c r="C93" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" spans="3:4">
       <c r="C94" s="13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="3:4">
       <c r="C95" s="13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="96" spans="3:4">
       <c r="C96" s="13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="3:4">
       <c r="C97" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" spans="3:4">
       <c r="C98" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="3:4">
       <c r="C99" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="100" spans="3:4">
       <c r="C100" s="13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="101" spans="3:4">
       <c r="C101" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="3:4">
       <c r="C102" s="13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="103" spans="3:4">
       <c r="C103" s="13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="104" spans="3:4">
       <c r="C104" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="105" spans="3:4">
       <c r="C105" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="106" spans="3:4">
       <c r="C106" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="107" spans="3:4">
       <c r="C107" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="108" spans="3:4">
       <c r="C108" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="109" spans="3:4">
       <c r="C109" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="110" spans="3:4">
       <c r="C110" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" spans="3:4">
       <c r="C111" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="3:4">
       <c r="C112" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="113" spans="3:4">
       <c r="C113" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="114" spans="3:4">
       <c r="C114" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115" spans="3:4">
       <c r="C115" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="116" spans="3:4">
       <c r="C116" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="117" spans="3:4">
       <c r="C117" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" spans="3:4">
       <c r="C118" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="119" spans="3:4">
       <c r="C119" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="120" spans="3:4">
       <c r="C120" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D120" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="121" spans="3:4">
       <c r="C121" s="13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="122" spans="3:4">
       <c r="C122" s="13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="123" spans="3:4">
       <c r="C123" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="124" spans="3:4">
       <c r="C124" s="13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="125" spans="3:4">
       <c r="C125" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="126" spans="3:4">
       <c r="C126" s="13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D126" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="127" spans="3:4">
       <c r="C127" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D127" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="128" spans="3:4">
       <c r="C128" s="13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="129" spans="3:4">
       <c r="C129" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D129" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="130" spans="3:4">
       <c r="C130" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D130" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="131" spans="3:4">
       <c r="C131" s="13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="132" spans="3:4">
       <c r="C132" s="13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D132" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="133" spans="3:4">
       <c r="C133" s="13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="134" spans="3:4">
       <c r="C134" s="13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D134" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="135" spans="3:4">
       <c r="C135" s="13" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D135" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="136" spans="3:4">
       <c r="C136" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="137" spans="3:4">
       <c r="C137" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D137" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="138" spans="3:4">
       <c r="C138" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D138" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="139" spans="3:4">
       <c r="C139" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="140" spans="3:4">
       <c r="C140" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="141" spans="3:4">
       <c r="C141" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D141" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="142" spans="3:4">
       <c r="C142" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D142" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="143" spans="3:4">
       <c r="C143" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="144" spans="3:4">
       <c r="C144" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="145" spans="3:4">
       <c r="C145" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="146" spans="3:4">
       <c r="C146" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="147" spans="3:4">
       <c r="C147" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="148" spans="3:4">
       <c r="C148" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D148" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="149" spans="3:4">
       <c r="C149" s="13" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D149" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="150" spans="3:4">
       <c r="C150" s="13" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D150" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="151" spans="3:4">
       <c r="C151" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="152" spans="3:4">
       <c r="C152" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="153" spans="3:4">
       <c r="C153" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="154" spans="3:4">
       <c r="C154" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="155" spans="3:4">
       <c r="C155" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D155" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="156" spans="3:4">
       <c r="C156" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D156" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="157" spans="3:4">
       <c r="C157" s="13" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="158" spans="3:4">
       <c r="C158" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="159" spans="3:4">
       <c r="C159" s="13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="160" spans="3:4">
       <c r="C160" s="13" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="161" spans="3:4">
       <c r="C161" s="13" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="162" spans="3:4">
       <c r="C162" s="13" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="163" spans="3:4">
       <c r="C163" s="13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="164" spans="3:4">
       <c r="C164" s="13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="165" spans="3:4">
       <c r="C165" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="166" spans="3:4">
       <c r="C166" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D166" s="14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="167" spans="3:4">
       <c r="C167" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D167" s="14" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="168" spans="3:4">
       <c r="C168" s="13" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="169" spans="3:4">
       <c r="C169" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="170" spans="3:4">
       <c r="C170" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D170" s="14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="171" spans="3:4">
       <c r="C171" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D171" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="172" spans="3:4">
       <c r="C172" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="173" spans="3:4">
       <c r="C173" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D173" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="174" spans="3:4">
       <c r="C174" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D174" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="175" spans="3:4">
       <c r="C175" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D175" s="14" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="176" spans="3:4">
       <c r="C176" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D176" s="14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="177" spans="3:4">
       <c r="C177" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D177" s="14" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="178" spans="3:4">
       <c r="C178" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D178" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="179" spans="3:4">
       <c r="C179" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D179" s="14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="180" spans="3:4">
       <c r="C180" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D180" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="181" spans="3:4">
       <c r="C181" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D181" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="182" spans="3:4">
       <c r="C182" s="13" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D182" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="183" spans="3:4">
       <c r="C183" s="13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D183" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="184" spans="3:4">
       <c r="C184" s="13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D184" s="14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="185" spans="3:4">
       <c r="C185" s="13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D185" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="186" spans="3:4">
       <c r="C186" s="13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D186" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="187" spans="3:4">
       <c r="C187" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D187" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="188" spans="3:4">
       <c r="C188" s="13" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="189" spans="3:4">
       <c r="C189" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="190" spans="3:4">
       <c r="C190" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="191" spans="3:4">
       <c r="C191" s="13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="192" spans="3:4">
       <c r="C192" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D192" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="193" spans="3:4">
       <c r="C193" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D193" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="194" spans="3:4">
       <c r="C194" s="13" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D194" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="195" spans="3:4">
       <c r="C195" s="13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D195" s="14" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="196" spans="3:4">
       <c r="C196" s="13" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D196" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="197" spans="3:4">
       <c r="C197" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D197" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="198" spans="3:4">
       <c r="C198" s="13" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D198" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="199" spans="3:4">
       <c r="C199" s="13" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D199" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="200" spans="3:4">
       <c r="C200" s="13" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D200" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="201" spans="3:4">
       <c r="C201" s="13" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D201" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="202" spans="3:4">
       <c r="C202" s="13" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D202" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="203" spans="3:4">
       <c r="C203" s="13" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D203" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="204" spans="3:4">
       <c r="C204" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D204" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="205" spans="3:4">
       <c r="C205" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D205" s="14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="206" spans="3:4">
       <c r="C206" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D206" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="207" spans="3:4">
       <c r="C207" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D207" s="14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="208" spans="3:4">
       <c r="C208" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D208" s="14" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="209" spans="3:4">
       <c r="C209" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D209" s="14" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="210" spans="3:4">
       <c r="C210" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D210" s="14" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="211" spans="3:4">
       <c r="C211" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D211" s="14" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="212" spans="3:4">
       <c r="C212" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D212" s="14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="213" spans="3:4">
       <c r="C213" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D213" s="14" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="214" spans="3:4">
       <c r="C214" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D214" s="14" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="215" spans="3:4">
       <c r="C215" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D215" s="14" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="216" spans="3:4">
       <c r="C216" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D216" s="14" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="217" spans="3:4">
       <c r="C217" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D217" s="14" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="218" spans="3:4">
       <c r="C218" s="13" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D218" s="14" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="219" spans="3:4">
       <c r="C219" s="13" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D219" s="14" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="220" spans="3:4">
       <c r="C220" s="13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D220" s="14" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="221" spans="3:4">
       <c r="C221" s="13" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D221" s="14" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="222" spans="3:4">
       <c r="C222" s="13" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D222" s="14" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="223" spans="3:4">
       <c r="C223" s="13" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D223" s="14" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="224" spans="3:4">
       <c r="C224" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D224" s="14" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="225" spans="3:4">
       <c r="C225" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D225" s="14" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="226" spans="3:4">
       <c r="C226" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D226" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="227" spans="3:4">
       <c r="C227" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D227" s="14" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="228" spans="3:4">
       <c r="C228" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D228" s="14" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="229" spans="3:4">
       <c r="C229" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D229" s="14" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="230" spans="3:4">
       <c r="C230" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D230" s="14" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="231" spans="3:4">
       <c r="C231" s="13" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D231" s="14" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="232" spans="3:4">
       <c r="C232" s="13" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D232" s="14" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="233" spans="3:4">
       <c r="C233" s="13" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D233" s="14" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="234" spans="3:4">
       <c r="C234" s="13" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D234" s="14" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="235" spans="3:4">
       <c r="C235" s="13" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D235" s="14" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="236" spans="3:4">
       <c r="C236" s="13" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D236" s="14" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="237" spans="3:4">
       <c r="C237" s="13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D237" s="14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="238" spans="3:4">
       <c r="C238" s="13" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D238" s="14" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="239" spans="3:4">
       <c r="C239" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D239" s="14" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="240" spans="3:4">
       <c r="C240" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D240" s="14" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="241" spans="3:4">
       <c r="C241" s="13" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D241" s="14" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="242" spans="3:4">
       <c r="C242" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D242" s="14" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="243" spans="3:4">
       <c r="C243" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D243" s="14" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="244" spans="3:4">
       <c r="C244" s="13" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D244" s="14" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="245" spans="3:4">
       <c r="C245" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D245" s="14" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="246" spans="3:4">
       <c r="C246" s="13" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D246" s="14" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="247" spans="3:4">
       <c r="C247" s="13" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D247" s="14" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="248" spans="3:4">
       <c r="C248" s="13" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D248" s="14" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="249" spans="3:4">
       <c r="C249" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D249" s="14" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="250" spans="3:4">
       <c r="C250" s="15" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D250" s="16" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IEN-870 create 'applied to bccnm' and 'complete ncas' milestone from spreadsheet (#584)
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD863759-8C45-6B4B-B6F1-992BE4358E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63930764-07AB-D44A-B008-1911F4D6EFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-780" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="542">
   <si>
     <t>Last Name</t>
   </si>
@@ -79,12 +79,6 @@
     <t>Zip/Postal Code</t>
   </si>
   <si>
-    <t>NCAS Asssessment Complete</t>
-  </si>
-  <si>
-    <t>BCCN Application Complete</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yes </t>
   </si>
   <si>
@@ -1664,6 +1658,12 @@
   </si>
   <si>
     <t>Robert.Frederick_648@acme.com</t>
+  </si>
+  <si>
+    <t>BCCNM Application Complete</t>
+  </si>
+  <si>
+    <t>NCAS Assessment Complete</t>
   </si>
 </sst>
 </file>
@@ -1943,8 +1943,8 @@
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[Country of Education]],Sheet1!C2:D250,2,0),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{A3485428-BB17-4719-9693-9A5D42422885}" name="Date ROS Contract Signed" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{C528BBBE-AF13-4DE4-8CB9-6A5D36322874}" name="NCAS Asssessment Complete" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{FC5EB113-2259-4AAD-B918-D66D8CDC1B70}" name="BCCN Application Complete" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{C528BBBE-AF13-4DE4-8CB9-6A5D36322874}" name="NCAS Assessment Complete" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{FC5EB113-2259-4AAD-B918-D66D8CDC1B70}" name="BCCNM Application Complete" dataDxfId="1"/>
     <tableColumn id="15" xr3:uid="{2EEE535B-18BF-4006-8377-F5D12DDCB956}" name="Registration Designation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2250,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2277,7 +2277,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -2304,22 +2304,22 @@
         <v>12</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>13</v>
+        <v>541</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>14</v>
+        <v>540</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -2327,22 +2327,28 @@
         <v>112374</v>
       </c>
       <c r="C2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>536</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>538</v>
-      </c>
       <c r="I2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="M2" s="9">
         <v>44562</v>
       </c>
+      <c r="N2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="P2" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2350,22 +2356,28 @@
         <v>111166</v>
       </c>
       <c r="C3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D3" t="s">
+        <v>531</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>533</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>535</v>
-      </c>
       <c r="I3" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="M3" s="9">
         <v>44593</v>
       </c>
+      <c r="N3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="P3" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -2373,19 +2385,19 @@
         <v>111208</v>
       </c>
       <c r="C4" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D4" t="s">
+        <v>537</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>539</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>541</v>
-      </c>
       <c r="I4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2393,19 +2405,19 @@
         <v>999999</v>
       </c>
       <c r="C5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D5" t="s">
+        <v>526</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>528</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>530</v>
-      </c>
       <c r="I5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -3042,7 +3054,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:O3 N4 N5:O59</xm:sqref>
+          <xm:sqref>N5:O59 O2:O3 N2:N4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41C196C3-3B03-4A85-A4EF-7D46FACB4C5B}">
           <x14:formula1>
@@ -3092,7 +3104,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -3175,2032 +3187,2032 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="C8" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="C10" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="C11" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="C12" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="C13" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="C14" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="C15" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="C16" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="3:4">
       <c r="C19" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="3:4">
       <c r="C20" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="3:4">
       <c r="C21" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="3:4">
       <c r="C22" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="3:4">
       <c r="C24" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="3:4">
       <c r="C25" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="3:4">
       <c r="C26" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="3:4">
       <c r="C27" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="3:4">
       <c r="C28" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="3:4">
       <c r="C29" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="3:4">
       <c r="C30" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="3:4">
       <c r="C31" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="3:4">
       <c r="C32" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="3:4">
       <c r="C81" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="3:4">
       <c r="C82" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="3:4">
       <c r="C83" s="13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="84" spans="3:4">
       <c r="C84" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="3:4">
       <c r="C85" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="86" spans="3:4">
       <c r="C86" s="13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="3:4">
       <c r="C87" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="88" spans="3:4">
       <c r="C88" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="89" spans="3:4">
       <c r="C89" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" spans="3:4">
       <c r="C90" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="91" spans="3:4">
       <c r="C91" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" spans="3:4">
       <c r="C92" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="93" spans="3:4">
       <c r="C93" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" spans="3:4">
       <c r="C94" s="13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="3:4">
       <c r="C95" s="13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="96" spans="3:4">
       <c r="C96" s="13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="3:4">
       <c r="C97" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" spans="3:4">
       <c r="C98" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="3:4">
       <c r="C99" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="100" spans="3:4">
       <c r="C100" s="13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="101" spans="3:4">
       <c r="C101" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="3:4">
       <c r="C102" s="13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="103" spans="3:4">
       <c r="C103" s="13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="104" spans="3:4">
       <c r="C104" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="105" spans="3:4">
       <c r="C105" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="106" spans="3:4">
       <c r="C106" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="107" spans="3:4">
       <c r="C107" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="108" spans="3:4">
       <c r="C108" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="109" spans="3:4">
       <c r="C109" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="110" spans="3:4">
       <c r="C110" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D110" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" spans="3:4">
       <c r="C111" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="3:4">
       <c r="C112" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="113" spans="3:4">
       <c r="C113" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="114" spans="3:4">
       <c r="C114" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115" spans="3:4">
       <c r="C115" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="116" spans="3:4">
       <c r="C116" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="117" spans="3:4">
       <c r="C117" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" spans="3:4">
       <c r="C118" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="119" spans="3:4">
       <c r="C119" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="120" spans="3:4">
       <c r="C120" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D120" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="121" spans="3:4">
       <c r="C121" s="13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D121" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="122" spans="3:4">
       <c r="C122" s="13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D122" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="123" spans="3:4">
       <c r="C123" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D123" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="124" spans="3:4">
       <c r="C124" s="13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="125" spans="3:4">
       <c r="C125" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="126" spans="3:4">
       <c r="C126" s="13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D126" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="127" spans="3:4">
       <c r="C127" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D127" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="128" spans="3:4">
       <c r="C128" s="13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D128" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="129" spans="3:4">
       <c r="C129" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D129" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="130" spans="3:4">
       <c r="C130" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D130" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="131" spans="3:4">
       <c r="C131" s="13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D131" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="132" spans="3:4">
       <c r="C132" s="13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D132" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="133" spans="3:4">
       <c r="C133" s="13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D133" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="134" spans="3:4">
       <c r="C134" s="13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D134" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="135" spans="3:4">
       <c r="C135" s="13" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D135" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="136" spans="3:4">
       <c r="C136" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D136" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="137" spans="3:4">
       <c r="C137" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D137" s="14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="138" spans="3:4">
       <c r="C138" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D138" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="139" spans="3:4">
       <c r="C139" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D139" s="14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="140" spans="3:4">
       <c r="C140" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D140" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="141" spans="3:4">
       <c r="C141" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D141" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="142" spans="3:4">
       <c r="C142" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D142" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="143" spans="3:4">
       <c r="C143" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D143" s="14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="144" spans="3:4">
       <c r="C144" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D144" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="145" spans="3:4">
       <c r="C145" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D145" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="146" spans="3:4">
       <c r="C146" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D146" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="147" spans="3:4">
       <c r="C147" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D147" s="14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="148" spans="3:4">
       <c r="C148" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D148" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="149" spans="3:4">
       <c r="C149" s="13" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D149" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="150" spans="3:4">
       <c r="C150" s="13" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D150" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="151" spans="3:4">
       <c r="C151" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="152" spans="3:4">
       <c r="C152" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D152" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="153" spans="3:4">
       <c r="C153" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D153" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="154" spans="3:4">
       <c r="C154" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D154" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="155" spans="3:4">
       <c r="C155" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D155" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="156" spans="3:4">
       <c r="C156" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D156" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="157" spans="3:4">
       <c r="C157" s="13" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D157" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="158" spans="3:4">
       <c r="C158" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D158" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="159" spans="3:4">
       <c r="C159" s="13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D159" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="160" spans="3:4">
       <c r="C160" s="13" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D160" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="161" spans="3:4">
       <c r="C161" s="13" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D161" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="162" spans="3:4">
       <c r="C162" s="13" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D162" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="163" spans="3:4">
       <c r="C163" s="13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D163" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="164" spans="3:4">
       <c r="C164" s="13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="165" spans="3:4">
       <c r="C165" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D165" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="166" spans="3:4">
       <c r="C166" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D166" s="14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="167" spans="3:4">
       <c r="C167" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D167" s="14" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="168" spans="3:4">
       <c r="C168" s="13" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="169" spans="3:4">
       <c r="C169" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="170" spans="3:4">
       <c r="C170" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D170" s="14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="171" spans="3:4">
       <c r="C171" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D171" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="172" spans="3:4">
       <c r="C172" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="173" spans="3:4">
       <c r="C173" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D173" s="14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="174" spans="3:4">
       <c r="C174" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D174" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="175" spans="3:4">
       <c r="C175" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D175" s="14" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="176" spans="3:4">
       <c r="C176" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D176" s="14" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="177" spans="3:4">
       <c r="C177" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D177" s="14" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="178" spans="3:4">
       <c r="C178" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D178" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="179" spans="3:4">
       <c r="C179" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D179" s="14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="180" spans="3:4">
       <c r="C180" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D180" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="181" spans="3:4">
       <c r="C181" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D181" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="182" spans="3:4">
       <c r="C182" s="13" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D182" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="183" spans="3:4">
       <c r="C183" s="13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D183" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="184" spans="3:4">
       <c r="C184" s="13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D184" s="14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="185" spans="3:4">
       <c r="C185" s="13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D185" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="186" spans="3:4">
       <c r="C186" s="13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D186" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="187" spans="3:4">
       <c r="C187" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D187" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="188" spans="3:4">
       <c r="C188" s="13" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D188" s="14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="189" spans="3:4">
       <c r="C189" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="190" spans="3:4">
       <c r="C190" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D190" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="191" spans="3:4">
       <c r="C191" s="13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D191" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="192" spans="3:4">
       <c r="C192" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D192" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="193" spans="3:4">
       <c r="C193" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D193" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="194" spans="3:4">
       <c r="C194" s="13" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D194" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="195" spans="3:4">
       <c r="C195" s="13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D195" s="14" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="196" spans="3:4">
       <c r="C196" s="13" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D196" s="14" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="197" spans="3:4">
       <c r="C197" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D197" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="198" spans="3:4">
       <c r="C198" s="13" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D198" s="14" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="199" spans="3:4">
       <c r="C199" s="13" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D199" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="200" spans="3:4">
       <c r="C200" s="13" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D200" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="201" spans="3:4">
       <c r="C201" s="13" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D201" s="14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="202" spans="3:4">
       <c r="C202" s="13" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D202" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="203" spans="3:4">
       <c r="C203" s="13" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D203" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="204" spans="3:4">
       <c r="C204" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D204" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="205" spans="3:4">
       <c r="C205" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D205" s="14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="206" spans="3:4">
       <c r="C206" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D206" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="207" spans="3:4">
       <c r="C207" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D207" s="14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="208" spans="3:4">
       <c r="C208" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D208" s="14" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="209" spans="3:4">
       <c r="C209" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D209" s="14" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="210" spans="3:4">
       <c r="C210" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D210" s="14" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="211" spans="3:4">
       <c r="C211" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D211" s="14" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="212" spans="3:4">
       <c r="C212" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D212" s="14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="213" spans="3:4">
       <c r="C213" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D213" s="14" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="214" spans="3:4">
       <c r="C214" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D214" s="14" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="215" spans="3:4">
       <c r="C215" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D215" s="14" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="216" spans="3:4">
       <c r="C216" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D216" s="14" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="217" spans="3:4">
       <c r="C217" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D217" s="14" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="218" spans="3:4">
       <c r="C218" s="13" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D218" s="14" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="219" spans="3:4">
       <c r="C219" s="13" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D219" s="14" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="220" spans="3:4">
       <c r="C220" s="13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D220" s="14" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="221" spans="3:4">
       <c r="C221" s="13" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D221" s="14" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="222" spans="3:4">
       <c r="C222" s="13" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D222" s="14" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="223" spans="3:4">
       <c r="C223" s="13" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D223" s="14" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="224" spans="3:4">
       <c r="C224" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D224" s="14" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="225" spans="3:4">
       <c r="C225" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D225" s="14" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="226" spans="3:4">
       <c r="C226" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D226" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="227" spans="3:4">
       <c r="C227" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D227" s="14" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="228" spans="3:4">
       <c r="C228" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D228" s="14" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="229" spans="3:4">
       <c r="C229" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D229" s="14" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="230" spans="3:4">
       <c r="C230" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D230" s="14" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="231" spans="3:4">
       <c r="C231" s="13" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D231" s="14" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="232" spans="3:4">
       <c r="C232" s="13" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D232" s="14" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="233" spans="3:4">
       <c r="C233" s="13" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D233" s="14" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="234" spans="3:4">
       <c r="C234" s="13" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D234" s="14" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="235" spans="3:4">
       <c r="C235" s="13" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D235" s="14" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="236" spans="3:4">
       <c r="C236" s="13" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D236" s="14" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="237" spans="3:4">
       <c r="C237" s="13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D237" s="14" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="238" spans="3:4">
       <c r="C238" s="13" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D238" s="14" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="239" spans="3:4">
       <c r="C239" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D239" s="14" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="240" spans="3:4">
       <c r="C240" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D240" s="14" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="241" spans="3:4">
       <c r="C241" s="13" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D241" s="14" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="242" spans="3:4">
       <c r="C242" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D242" s="14" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="243" spans="3:4">
       <c r="C243" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D243" s="14" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="244" spans="3:4">
       <c r="C244" s="13" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D244" s="14" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="245" spans="3:4">
       <c r="C245" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D245" s="14" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="246" spans="3:4">
       <c r="C246" s="13" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D246" s="14" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="247" spans="3:4">
       <c r="C247" s="13" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D247" s="14" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="248" spans="3:4">
       <c r="C248" s="13" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D248" s="14" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="249" spans="3:4">
       <c r="C249" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D249" s="14" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="250" spans="3:4">
       <c r="C250" s="15" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D250" s="16" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IEN-873 ATS does not overwrite ROS by BCCNM/NCAS spreadsheet
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63930764-07AB-D44A-B008-1911F4D6EFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8536932E-B898-0C4B-9390-02DFE6EADC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-780" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="542">
   <si>
     <t>Last Name</t>
   </si>
@@ -2250,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2341,8 +2341,8 @@
       <c r="M2" s="9">
         <v>44562</v>
       </c>
-      <c r="N2" s="11" t="s">
-        <v>13</v>
+      <c r="N2" s="9">
+        <v>44563</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>13</v>
@@ -2370,8 +2370,8 @@
       <c r="M3" s="9">
         <v>44593</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>13</v>
+      <c r="N3" s="9">
+        <v>44594</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>13</v>
@@ -2396,6 +2396,9 @@
       <c r="I4" t="s">
         <v>530</v>
       </c>
+      <c r="O4" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="P4" s="11" t="s">
         <v>524</v>
       </c>
@@ -2416,6 +2419,12 @@
       <c r="I5" t="s">
         <v>525</v>
       </c>
+      <c r="N5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="P5" s="11" t="s">
         <v>20</v>
       </c>
@@ -2424,10 +2433,16 @@
       <c r="M6" s="9">
         <v>44562</v>
       </c>
+      <c r="O6" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
       <c r="M7" s="9">
         <v>44593</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="11" customFormat="1">
@@ -3033,7 +3048,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:P1" xr:uid="{BEEEE0E7-8791-4CC6-B23A-AAB276F68531}"/>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M60:O1048576 M2:M59" xr:uid="{FC76C5EB-0027-4C81-9F77-08421AE0CD39}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M60:O1048576 M2:M59 N2:N3" xr:uid="{FC76C5EB-0027-4C81-9F77-08421AE0CD39}">
       <formula1>43831</formula1>
     </dataValidation>
   </dataValidations>
@@ -3054,7 +3069,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>N5:O59 O2:O3 N2:N4</xm:sqref>
+          <xm:sqref>O2:O3 N4:O59</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41C196C3-3B03-4A85-A4EF-7D46FACB4C5B}">
           <x14:formula1>

</xml_diff>

<commit_message>
IEN-873 feedback bccnm ncas updates (#590)
* IEN-873 ATS does not overwrite ROS by BCCNM/NCAS spreadsheet
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63930764-07AB-D44A-B008-1911F4D6EFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8536932E-B898-0C4B-9390-02DFE6EADC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-780" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="542">
   <si>
     <t>Last Name</t>
   </si>
@@ -2250,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2341,8 +2341,8 @@
       <c r="M2" s="9">
         <v>44562</v>
       </c>
-      <c r="N2" s="11" t="s">
-        <v>13</v>
+      <c r="N2" s="9">
+        <v>44563</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>13</v>
@@ -2370,8 +2370,8 @@
       <c r="M3" s="9">
         <v>44593</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>13</v>
+      <c r="N3" s="9">
+        <v>44594</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>13</v>
@@ -2396,6 +2396,9 @@
       <c r="I4" t="s">
         <v>530</v>
       </c>
+      <c r="O4" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="P4" s="11" t="s">
         <v>524</v>
       </c>
@@ -2416,6 +2419,12 @@
       <c r="I5" t="s">
         <v>525</v>
       </c>
+      <c r="N5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="P5" s="11" t="s">
         <v>20</v>
       </c>
@@ -2424,10 +2433,16 @@
       <c r="M6" s="9">
         <v>44562</v>
       </c>
+      <c r="O6" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
       <c r="M7" s="9">
         <v>44593</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="11" customFormat="1">
@@ -3033,7 +3048,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:P1" xr:uid="{BEEEE0E7-8791-4CC6-B23A-AAB276F68531}"/>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M60:O1048576 M2:M59" xr:uid="{FC76C5EB-0027-4C81-9F77-08421AE0CD39}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M60:O1048576 M2:M59 N2:N3" xr:uid="{FC76C5EB-0027-4C81-9F77-08421AE0CD39}">
       <formula1>43831</formula1>
     </dataValidation>
   </dataValidations>
@@ -3054,7 +3069,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>N5:O59 O2:O3 N2:N4</xm:sqref>
+          <xm:sqref>O2:O3 N4:O59</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41C196C3-3B03-4A85-A4EF-7D46FACB4C5B}">
           <x14:formula1>

</xml_diff>

<commit_message>
IEN-879 add education country from bccnm spreadsheet
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8536932E-B898-0C4B-9390-02DFE6EADC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15588D6E-998E-8347-9397-827BAD622748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-780" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
+    <workbookView xWindow="9960" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Template - DO NOT EDIT" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="546">
   <si>
     <t>Last Name</t>
   </si>
@@ -1664,6 +1664,18 @@
   </si>
   <si>
     <t>NCAS Assessment Complete</t>
+  </si>
+  <si>
+    <t>Begue</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
+    <t>Trevor.Begue_784@gmail.com</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -2250,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2338,6 +2350,9 @@
       <c r="I2" t="s">
         <v>529</v>
       </c>
+      <c r="K2" t="s">
+        <v>529</v>
+      </c>
       <c r="M2" s="9">
         <v>44562</v>
       </c>
@@ -2367,6 +2382,9 @@
       <c r="I3" t="s">
         <v>529</v>
       </c>
+      <c r="K3" t="s">
+        <v>529</v>
+      </c>
       <c r="M3" s="9">
         <v>44593</v>
       </c>
@@ -2396,6 +2414,7 @@
       <c r="I4" t="s">
         <v>530</v>
       </c>
+      <c r="N4" s="9"/>
       <c r="O4" s="11" t="s">
         <v>14</v>
       </c>
@@ -2405,20 +2424,23 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
-        <v>999999</v>
+        <v>111631</v>
       </c>
       <c r="C5" t="s">
-        <v>527</v>
+        <v>542</v>
       </c>
       <c r="D5" t="s">
-        <v>526</v>
+        <v>543</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>528</v>
+        <v>544</v>
       </c>
       <c r="I5" t="s">
         <v>525</v>
       </c>
+      <c r="K5" t="s">
+        <v>545</v>
+      </c>
       <c r="N5" s="11" t="s">
         <v>14</v>
       </c>
@@ -2430,11 +2452,32 @@
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="M6" s="9">
-        <v>44562</v>
+      <c r="A6">
+        <v>999999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>527</v>
+      </c>
+      <c r="D6" t="s">
+        <v>526</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>528</v>
+      </c>
+      <c r="I6" t="s">
+        <v>525</v>
+      </c>
+      <c r="K6" t="s">
+        <v>525</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="O6" s="11" t="s">
         <v>14</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3048,7 +3091,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:P1" xr:uid="{BEEEE0E7-8791-4CC6-B23A-AAB276F68531}"/>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M60:O1048576 M2:M59 N2:N3" xr:uid="{FC76C5EB-0027-4C81-9F77-08421AE0CD39}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M60:O1048576 N2:N4 M2:M59" xr:uid="{FC76C5EB-0027-4C81-9F77-08421AE0CD39}">
       <formula1>43831</formula1>
     </dataValidation>
   </dataValidations>
@@ -3056,11 +3099,12 @@
     <hyperlink ref="E3" r:id="rId1" xr:uid="{E3945063-52D5-A548-8EA5-6BD94A59966E}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{EA489891-52B7-5D45-9F5B-A7DA4212960F}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{86D5D6EE-2985-2F41-A4C4-8D6C4D808E3B}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{D9C29F5B-E5C6-4D4A-BF7A-7271A2373F1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -3069,7 +3113,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O3 N4:O59</xm:sqref>
+          <xm:sqref>O2:O59 N5:N59</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41C196C3-3B03-4A85-A4EF-7D46FACB4C5B}">
           <x14:formula1>
@@ -3081,7 +3125,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$C$2:$C$250</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>K7:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
IEN-879 add education country from bccnm spreadsheet (#604)
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8536932E-B898-0C4B-9390-02DFE6EADC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15588D6E-998E-8347-9397-827BAD622748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-780" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
+    <workbookView xWindow="9960" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Template - DO NOT EDIT" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="546">
   <si>
     <t>Last Name</t>
   </si>
@@ -1664,6 +1664,18 @@
   </si>
   <si>
     <t>NCAS Assessment Complete</t>
+  </si>
+  <si>
+    <t>Begue</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
+    <t>Trevor.Begue_784@gmail.com</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -2250,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2338,6 +2350,9 @@
       <c r="I2" t="s">
         <v>529</v>
       </c>
+      <c r="K2" t="s">
+        <v>529</v>
+      </c>
       <c r="M2" s="9">
         <v>44562</v>
       </c>
@@ -2367,6 +2382,9 @@
       <c r="I3" t="s">
         <v>529</v>
       </c>
+      <c r="K3" t="s">
+        <v>529</v>
+      </c>
       <c r="M3" s="9">
         <v>44593</v>
       </c>
@@ -2396,6 +2414,7 @@
       <c r="I4" t="s">
         <v>530</v>
       </c>
+      <c r="N4" s="9"/>
       <c r="O4" s="11" t="s">
         <v>14</v>
       </c>
@@ -2405,20 +2424,23 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
-        <v>999999</v>
+        <v>111631</v>
       </c>
       <c r="C5" t="s">
-        <v>527</v>
+        <v>542</v>
       </c>
       <c r="D5" t="s">
-        <v>526</v>
+        <v>543</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>528</v>
+        <v>544</v>
       </c>
       <c r="I5" t="s">
         <v>525</v>
       </c>
+      <c r="K5" t="s">
+        <v>545</v>
+      </c>
       <c r="N5" s="11" t="s">
         <v>14</v>
       </c>
@@ -2430,11 +2452,32 @@
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="M6" s="9">
-        <v>44562</v>
+      <c r="A6">
+        <v>999999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>527</v>
+      </c>
+      <c r="D6" t="s">
+        <v>526</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>528</v>
+      </c>
+      <c r="I6" t="s">
+        <v>525</v>
+      </c>
+      <c r="K6" t="s">
+        <v>525</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="O6" s="11" t="s">
         <v>14</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3048,7 +3091,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:P1" xr:uid="{BEEEE0E7-8791-4CC6-B23A-AAB276F68531}"/>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M60:O1048576 M2:M59 N2:N3" xr:uid="{FC76C5EB-0027-4C81-9F77-08421AE0CD39}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M60:O1048576 N2:N4 M2:M59" xr:uid="{FC76C5EB-0027-4C81-9F77-08421AE0CD39}">
       <formula1>43831</formula1>
     </dataValidation>
   </dataValidations>
@@ -3056,11 +3099,12 @@
     <hyperlink ref="E3" r:id="rId1" xr:uid="{E3945063-52D5-A548-8EA5-6BD94A59966E}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{EA489891-52B7-5D45-9F5B-A7DA4212960F}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{86D5D6EE-2985-2F41-A4C4-8D6C4D808E3B}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{D9C29F5B-E5C6-4D4A-BF7A-7271A2373F1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -3069,7 +3113,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O3 N4:O59</xm:sqref>
+          <xm:sqref>O2:O59 N5:N59</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41C196C3-3B03-4A85-A4EF-7D46FACB4C5B}">
           <x14:formula1>
@@ -3081,7 +3125,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$C$2:$C$250</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>K7:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
update xlsx file to new column
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eycanada-my.sharepoint.com/personal/jerry_wang_ca_ey_com/Documents/Documents/projects/jerry/internationally-educated-nurses/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15588D6E-998E-8347-9397-827BAD622748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{15588D6E-998E-8347-9397-827BAD622748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C70F60A-646A-8C4C-A3F5-32B9362E166B}"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20360" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Template - DO NOT EDIT" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Country of Education</t>
-  </si>
-  <si>
     <t>Registration Designation</t>
   </si>
   <si>
@@ -1676,6 +1673,9 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>ISO Code - Education</t>
   </si>
 </sst>
 </file>
@@ -1950,9 +1950,9 @@
     <tableColumn id="9" xr3:uid="{C29B86CB-35D1-4A90-988C-B376D1F11746}" name="State/Province" dataDxfId="5"/>
     <tableColumn id="10" xr3:uid="{51680233-1ACB-4042-AB01-CF531A1CA912}" name="Country"/>
     <tableColumn id="11" xr3:uid="{7CBE1023-D597-4113-A0E3-6BF724D0B2F5}" name="Zip/Postal Code"/>
-    <tableColumn id="14" xr3:uid="{B2EE4131-382E-447B-8582-93712B4E1CE0}" name="Country of Education"/>
+    <tableColumn id="14" xr3:uid="{B2EE4131-382E-447B-8582-93712B4E1CE0}" name="ISO Code - Education"/>
     <tableColumn id="13" xr3:uid="{312FBB00-E05F-4292-8BE8-67886879CB82}" name="ISO Code" dataDxfId="4">
-      <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[Country of Education]],Sheet1!C2:D250,2,0),"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[ISO Code - Education]],Sheet1!C2:D250,2,0),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{A3485428-BB17-4719-9693-9A5D42422885}" name="Date ROS Contract Signed" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{C528BBBE-AF13-4DE4-8CB9-6A5D36322874}" name="NCAS Assessment Complete" dataDxfId="2"/>
@@ -1964,9 +1964,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2004,7 +2004,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2110,7 +2110,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2252,7 +2252,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2262,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:N4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2289,7 +2289,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -2316,22 +2316,22 @@
         <v>12</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>15</v>
+        <v>545</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -2339,19 +2339,19 @@
         <v>112374</v>
       </c>
       <c r="C2" t="s">
+        <v>534</v>
+      </c>
+      <c r="D2" t="s">
+        <v>533</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>535</v>
       </c>
-      <c r="D2" t="s">
-        <v>534</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>536</v>
-      </c>
       <c r="I2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="M2" s="9">
         <v>44562</v>
@@ -2363,7 +2363,7 @@
         <v>13</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2371,19 +2371,19 @@
         <v>111166</v>
       </c>
       <c r="C3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D3" t="s">
+        <v>530</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>532</v>
       </c>
-      <c r="D3" t="s">
-        <v>531</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>533</v>
-      </c>
       <c r="I3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="M3" s="9">
         <v>44593</v>
@@ -2395,7 +2395,7 @@
         <v>13</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -2403,23 +2403,23 @@
         <v>111208</v>
       </c>
       <c r="C4" t="s">
+        <v>537</v>
+      </c>
+      <c r="D4" t="s">
+        <v>536</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>538</v>
       </c>
-      <c r="D4" t="s">
-        <v>537</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>539</v>
-      </c>
       <c r="I4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="N4" s="9"/>
       <c r="O4" s="11" t="s">
         <v>14</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2427,19 +2427,19 @@
         <v>111631</v>
       </c>
       <c r="C5" t="s">
+        <v>541</v>
+      </c>
+      <c r="D5" t="s">
         <v>542</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="17" t="s">
         <v>543</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="I5" t="s">
+        <v>524</v>
+      </c>
+      <c r="K5" t="s">
         <v>544</v>
-      </c>
-      <c r="I5" t="s">
-        <v>525</v>
-      </c>
-      <c r="K5" t="s">
-        <v>545</v>
       </c>
       <c r="N5" s="11" t="s">
         <v>14</v>
@@ -2448,7 +2448,7 @@
         <v>14</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -2456,19 +2456,19 @@
         <v>999999</v>
       </c>
       <c r="C6" t="s">
+        <v>526</v>
+      </c>
+      <c r="D6" t="s">
+        <v>525</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>527</v>
       </c>
-      <c r="D6" t="s">
-        <v>526</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>528</v>
-      </c>
       <c r="I6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="N6" s="11" t="s">
         <v>14</v>
@@ -2477,7 +2477,7 @@
         <v>14</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3163,7 +3163,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -3246,16 +3246,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>522</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3263,13 +3263,13 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3277,2001 +3277,2001 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="C8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="C10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="C11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="C12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="C13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="C14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="C15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="C16" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="3:4">
       <c r="C19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="3:4">
       <c r="C20" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="3:4">
       <c r="C21" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="3:4">
       <c r="C22" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>67</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="3:4">
       <c r="C24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="3:4">
       <c r="C25" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="3:4">
       <c r="C26" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="27" spans="3:4">
       <c r="C27" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="28" spans="3:4">
       <c r="C28" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="29" spans="3:4">
       <c r="C29" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="30" spans="3:4">
       <c r="C30" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="31" spans="3:4">
       <c r="C31" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="3:4">
       <c r="C32" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="14" t="s">
         <v>85</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="14" t="s">
         <v>87</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>91</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>101</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>107</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" s="14" t="s">
         <v>123</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55" s="14" t="s">
         <v>131</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D56" s="14" t="s">
         <v>133</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>137</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>139</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D61" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D63" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D64" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" s="14" t="s">
         <v>151</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D67" s="14" t="s">
         <v>155</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D68" s="14" t="s">
         <v>157</v>
-      </c>
-      <c r="D68" s="14" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D69" s="14" t="s">
         <v>159</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D70" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D71" s="14" t="s">
         <v>163</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D72" s="14" t="s">
         <v>165</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D73" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D74" s="14" t="s">
         <v>169</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D75" s="14" t="s">
         <v>171</v>
-      </c>
-      <c r="D75" s="14" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D76" s="14" t="s">
         <v>173</v>
-      </c>
-      <c r="D76" s="14" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D77" s="14" t="s">
         <v>175</v>
-      </c>
-      <c r="D77" s="14" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D78" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="D78" s="14" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D79" s="14" t="s">
         <v>179</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D80" s="14" t="s">
         <v>181</v>
-      </c>
-      <c r="D80" s="14" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="81" spans="3:4">
       <c r="C81" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D81" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="82" spans="3:4">
       <c r="C82" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D82" s="14" t="s">
         <v>185</v>
-      </c>
-      <c r="D82" s="14" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="83" spans="3:4">
       <c r="C83" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D83" s="14" t="s">
         <v>187</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="84" spans="3:4">
       <c r="C84" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D84" s="14" t="s">
         <v>189</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="85" spans="3:4">
       <c r="C85" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D85" s="14" t="s">
         <v>191</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="86" spans="3:4">
       <c r="C86" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D86" s="14" t="s">
         <v>193</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="87" spans="3:4">
       <c r="C87" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" s="14" t="s">
         <v>195</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="88" spans="3:4">
       <c r="C88" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D88" s="14" t="s">
         <v>197</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="89" spans="3:4">
       <c r="C89" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D89" s="14" t="s">
         <v>199</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="90" spans="3:4">
       <c r="C90" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D90" s="14" t="s">
         <v>201</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="91" spans="3:4">
       <c r="C91" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D91" s="14" t="s">
         <v>203</v>
-      </c>
-      <c r="D91" s="14" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="92" spans="3:4">
       <c r="C92" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D92" s="14" t="s">
         <v>205</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="93" spans="3:4">
       <c r="C93" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="D93" s="14" t="s">
         <v>207</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="94" spans="3:4">
       <c r="C94" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D94" s="14" t="s">
         <v>209</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="95" spans="3:4">
       <c r="C95" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D95" s="14" t="s">
         <v>211</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="96" spans="3:4">
       <c r="C96" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="D96" s="14" t="s">
         <v>213</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="97" spans="3:4">
       <c r="C97" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D97" s="14" t="s">
         <v>215</v>
-      </c>
-      <c r="D97" s="14" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="98" spans="3:4">
       <c r="C98" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D98" s="14" t="s">
         <v>217</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="99" spans="3:4">
       <c r="C99" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D99" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="D99" s="14" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="100" spans="3:4">
       <c r="C100" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D100" s="14" t="s">
         <v>221</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="101" spans="3:4">
       <c r="C101" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D101" s="14" t="s">
         <v>223</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="102" spans="3:4">
       <c r="C102" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D102" s="14" t="s">
         <v>225</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="103" spans="3:4">
       <c r="C103" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D103" s="14" t="s">
         <v>227</v>
-      </c>
-      <c r="D103" s="14" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="104" spans="3:4">
       <c r="C104" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D104" s="14" t="s">
         <v>229</v>
-      </c>
-      <c r="D104" s="14" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="105" spans="3:4">
       <c r="C105" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D105" s="14" t="s">
         <v>231</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="106" spans="3:4">
       <c r="C106" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D106" s="14" t="s">
         <v>233</v>
-      </c>
-      <c r="D106" s="14" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="107" spans="3:4">
       <c r="C107" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D107" s="14" t="s">
         <v>235</v>
-      </c>
-      <c r="D107" s="14" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="108" spans="3:4">
       <c r="C108" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D108" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="D108" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="109" spans="3:4">
       <c r="C109" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D109" s="14" t="s">
         <v>239</v>
-      </c>
-      <c r="D109" s="14" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="110" spans="3:4">
       <c r="C110" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D110" s="14" t="s">
         <v>241</v>
-      </c>
-      <c r="D110" s="14" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="111" spans="3:4">
       <c r="C111" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D111" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="D111" s="14" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="112" spans="3:4">
       <c r="C112" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D112" s="14" t="s">
         <v>245</v>
-      </c>
-      <c r="D112" s="14" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="113" spans="3:4">
       <c r="C113" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="D113" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="D113" s="14" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="114" spans="3:4">
       <c r="C114" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D114" s="14" t="s">
         <v>249</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="115" spans="3:4">
       <c r="C115" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D115" s="14" t="s">
         <v>251</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="116" spans="3:4">
       <c r="C116" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D116" s="14" t="s">
         <v>253</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="117" spans="3:4">
       <c r="C117" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D117" s="14" t="s">
         <v>255</v>
-      </c>
-      <c r="D117" s="14" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="118" spans="3:4">
       <c r="C118" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="D118" s="14" t="s">
         <v>257</v>
-      </c>
-      <c r="D118" s="14" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="119" spans="3:4">
       <c r="C119" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="D119" s="14" t="s">
         <v>259</v>
-      </c>
-      <c r="D119" s="14" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="120" spans="3:4">
       <c r="C120" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D120" s="14" t="s">
         <v>261</v>
-      </c>
-      <c r="D120" s="14" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="121" spans="3:4">
       <c r="C121" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D121" s="14" t="s">
         <v>263</v>
-      </c>
-      <c r="D121" s="14" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="122" spans="3:4">
       <c r="C122" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D122" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="D122" s="14" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="123" spans="3:4">
       <c r="C123" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D123" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="D123" s="14" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="124" spans="3:4">
       <c r="C124" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D124" s="14" t="s">
         <v>269</v>
-      </c>
-      <c r="D124" s="14" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="125" spans="3:4">
       <c r="C125" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D125" s="14" t="s">
         <v>271</v>
-      </c>
-      <c r="D125" s="14" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="126" spans="3:4">
       <c r="C126" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D126" s="14" t="s">
         <v>273</v>
-      </c>
-      <c r="D126" s="14" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="127" spans="3:4">
       <c r="C127" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="D127" s="14" t="s">
         <v>275</v>
-      </c>
-      <c r="D127" s="14" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="128" spans="3:4">
       <c r="C128" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D128" s="14" t="s">
         <v>277</v>
-      </c>
-      <c r="D128" s="14" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="129" spans="3:4">
       <c r="C129" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D129" s="14" t="s">
         <v>279</v>
-      </c>
-      <c r="D129" s="14" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="130" spans="3:4">
       <c r="C130" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="D130" s="14" t="s">
         <v>281</v>
-      </c>
-      <c r="D130" s="14" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="131" spans="3:4">
       <c r="C131" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D131" s="14" t="s">
         <v>283</v>
-      </c>
-      <c r="D131" s="14" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="132" spans="3:4">
       <c r="C132" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D132" s="14" t="s">
         <v>285</v>
-      </c>
-      <c r="D132" s="14" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="133" spans="3:4">
       <c r="C133" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D133" s="14" t="s">
         <v>287</v>
-      </c>
-      <c r="D133" s="14" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="134" spans="3:4">
       <c r="C134" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="D134" s="14" t="s">
         <v>289</v>
-      </c>
-      <c r="D134" s="14" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="135" spans="3:4">
       <c r="C135" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D135" s="14" t="s">
         <v>291</v>
-      </c>
-      <c r="D135" s="14" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="136" spans="3:4">
       <c r="C136" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="D136" s="14" t="s">
         <v>293</v>
-      </c>
-      <c r="D136" s="14" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="137" spans="3:4">
       <c r="C137" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D137" s="14" t="s">
         <v>295</v>
-      </c>
-      <c r="D137" s="14" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="138" spans="3:4">
       <c r="C138" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="D138" s="14" t="s">
         <v>297</v>
-      </c>
-      <c r="D138" s="14" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="139" spans="3:4">
       <c r="C139" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="D139" s="14" t="s">
         <v>299</v>
-      </c>
-      <c r="D139" s="14" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="140" spans="3:4">
       <c r="C140" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D140" s="14" t="s">
         <v>301</v>
-      </c>
-      <c r="D140" s="14" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="141" spans="3:4">
       <c r="C141" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D141" s="14" t="s">
         <v>303</v>
-      </c>
-      <c r="D141" s="14" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="142" spans="3:4">
       <c r="C142" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="D142" s="14" t="s">
         <v>305</v>
-      </c>
-      <c r="D142" s="14" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="143" spans="3:4">
       <c r="C143" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="D143" s="14" t="s">
         <v>307</v>
-      </c>
-      <c r="D143" s="14" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="144" spans="3:4">
       <c r="C144" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="D144" s="14" t="s">
         <v>309</v>
-      </c>
-      <c r="D144" s="14" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="145" spans="3:4">
       <c r="C145" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D145" s="14" t="s">
         <v>311</v>
-      </c>
-      <c r="D145" s="14" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="146" spans="3:4">
       <c r="C146" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="D146" s="14" t="s">
         <v>313</v>
-      </c>
-      <c r="D146" s="14" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="147" spans="3:4">
       <c r="C147" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="D147" s="14" t="s">
         <v>315</v>
-      </c>
-      <c r="D147" s="14" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="148" spans="3:4">
       <c r="C148" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D148" s="14" t="s">
         <v>317</v>
-      </c>
-      <c r="D148" s="14" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="149" spans="3:4">
       <c r="C149" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="D149" s="14" t="s">
         <v>319</v>
-      </c>
-      <c r="D149" s="14" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="150" spans="3:4">
       <c r="C150" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="D150" s="14" t="s">
         <v>321</v>
-      </c>
-      <c r="D150" s="14" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="151" spans="3:4">
       <c r="C151" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="D151" s="14" t="s">
         <v>323</v>
-      </c>
-      <c r="D151" s="14" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="152" spans="3:4">
       <c r="C152" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="D152" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="D152" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="153" spans="3:4">
       <c r="C153" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="D153" s="14" t="s">
         <v>327</v>
-      </c>
-      <c r="D153" s="14" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="154" spans="3:4">
       <c r="C154" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="D154" s="14" t="s">
         <v>329</v>
-      </c>
-      <c r="D154" s="14" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="155" spans="3:4">
       <c r="C155" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="D155" s="14" t="s">
         <v>331</v>
-      </c>
-      <c r="D155" s="14" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="156" spans="3:4">
       <c r="C156" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="D156" s="14" t="s">
         <v>333</v>
-      </c>
-      <c r="D156" s="14" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="157" spans="3:4">
       <c r="C157" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="D157" s="14" t="s">
         <v>335</v>
-      </c>
-      <c r="D157" s="14" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="158" spans="3:4">
       <c r="C158" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="D158" s="14" t="s">
         <v>337</v>
-      </c>
-      <c r="D158" s="14" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="159" spans="3:4">
       <c r="C159" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="D159" s="14" t="s">
         <v>339</v>
-      </c>
-      <c r="D159" s="14" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="160" spans="3:4">
       <c r="C160" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="D160" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="D160" s="14" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="161" spans="3:4">
       <c r="C161" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D161" s="14" t="s">
         <v>343</v>
-      </c>
-      <c r="D161" s="14" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="162" spans="3:4">
       <c r="C162" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="D162" s="14" t="s">
         <v>345</v>
-      </c>
-      <c r="D162" s="14" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="163" spans="3:4">
       <c r="C163" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="D163" s="14" t="s">
         <v>347</v>
-      </c>
-      <c r="D163" s="14" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="164" spans="3:4">
       <c r="C164" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="D164" s="14" t="s">
         <v>349</v>
-      </c>
-      <c r="D164" s="14" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="165" spans="3:4">
       <c r="C165" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="D165" s="14" t="s">
         <v>351</v>
-      </c>
-      <c r="D165" s="14" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="166" spans="3:4">
       <c r="C166" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="D166" s="14" t="s">
         <v>353</v>
-      </c>
-      <c r="D166" s="14" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="167" spans="3:4">
       <c r="C167" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="D167" s="14" t="s">
         <v>355</v>
-      </c>
-      <c r="D167" s="14" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="168" spans="3:4">
       <c r="C168" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="D168" s="14" t="s">
         <v>357</v>
-      </c>
-      <c r="D168" s="14" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="169" spans="3:4">
       <c r="C169" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="D169" s="14" t="s">
         <v>359</v>
-      </c>
-      <c r="D169" s="14" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="170" spans="3:4">
       <c r="C170" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="D170" s="14" t="s">
         <v>361</v>
-      </c>
-      <c r="D170" s="14" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="171" spans="3:4">
       <c r="C171" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="D171" s="14" t="s">
         <v>363</v>
-      </c>
-      <c r="D171" s="14" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="172" spans="3:4">
       <c r="C172" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="D172" s="14" t="s">
         <v>365</v>
-      </c>
-      <c r="D172" s="14" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="173" spans="3:4">
       <c r="C173" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="D173" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="D173" s="14" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="174" spans="3:4">
       <c r="C174" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="D174" s="14" t="s">
         <v>369</v>
-      </c>
-      <c r="D174" s="14" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="175" spans="3:4">
       <c r="C175" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="D175" s="14" t="s">
         <v>371</v>
-      </c>
-      <c r="D175" s="14" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="176" spans="3:4">
       <c r="C176" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="D176" s="14" t="s">
         <v>373</v>
-      </c>
-      <c r="D176" s="14" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="177" spans="3:4">
       <c r="C177" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D177" s="14" t="s">
         <v>375</v>
-      </c>
-      <c r="D177" s="14" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="178" spans="3:4">
       <c r="C178" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="D178" s="14" t="s">
         <v>377</v>
-      </c>
-      <c r="D178" s="14" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="179" spans="3:4">
       <c r="C179" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="D179" s="14" t="s">
         <v>379</v>
-      </c>
-      <c r="D179" s="14" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="180" spans="3:4">
       <c r="C180" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="D180" s="14" t="s">
         <v>381</v>
-      </c>
-      <c r="D180" s="14" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="181" spans="3:4">
       <c r="C181" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="D181" s="14" t="s">
         <v>383</v>
-      </c>
-      <c r="D181" s="14" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="182" spans="3:4">
       <c r="C182" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="D182" s="14" t="s">
         <v>385</v>
-      </c>
-      <c r="D182" s="14" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="183" spans="3:4">
       <c r="C183" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D183" s="14" t="s">
         <v>387</v>
-      </c>
-      <c r="D183" s="14" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="184" spans="3:4">
       <c r="C184" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="D184" s="14" t="s">
         <v>389</v>
-      </c>
-      <c r="D184" s="14" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="185" spans="3:4">
       <c r="C185" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="D185" s="14" t="s">
         <v>391</v>
-      </c>
-      <c r="D185" s="14" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="186" spans="3:4">
       <c r="C186" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="D186" s="14" t="s">
         <v>393</v>
-      </c>
-      <c r="D186" s="14" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="187" spans="3:4">
       <c r="C187" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="D187" s="14" t="s">
         <v>395</v>
-      </c>
-      <c r="D187" s="14" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="188" spans="3:4">
       <c r="C188" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="D188" s="14" t="s">
         <v>397</v>
-      </c>
-      <c r="D188" s="14" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="189" spans="3:4">
       <c r="C189" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="D189" s="14" t="s">
         <v>399</v>
-      </c>
-      <c r="D189" s="14" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="190" spans="3:4">
       <c r="C190" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="D190" s="14" t="s">
         <v>401</v>
-      </c>
-      <c r="D190" s="14" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="191" spans="3:4">
       <c r="C191" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="D191" s="14" t="s">
         <v>403</v>
-      </c>
-      <c r="D191" s="14" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="192" spans="3:4">
       <c r="C192" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="D192" s="14" t="s">
         <v>405</v>
-      </c>
-      <c r="D192" s="14" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="193" spans="3:4">
       <c r="C193" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="D193" s="14" t="s">
         <v>407</v>
-      </c>
-      <c r="D193" s="14" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="194" spans="3:4">
       <c r="C194" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="D194" s="14" t="s">
         <v>409</v>
-      </c>
-      <c r="D194" s="14" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="195" spans="3:4">
       <c r="C195" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="D195" s="14" t="s">
         <v>411</v>
-      </c>
-      <c r="D195" s="14" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="196" spans="3:4">
       <c r="C196" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="D196" s="14" t="s">
         <v>413</v>
-      </c>
-      <c r="D196" s="14" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="197" spans="3:4">
       <c r="C197" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="D197" s="14" t="s">
         <v>415</v>
-      </c>
-      <c r="D197" s="14" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="198" spans="3:4">
       <c r="C198" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="D198" s="14" t="s">
         <v>417</v>
-      </c>
-      <c r="D198" s="14" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="199" spans="3:4">
       <c r="C199" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="D199" s="14" t="s">
         <v>419</v>
-      </c>
-      <c r="D199" s="14" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="200" spans="3:4">
       <c r="C200" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="D200" s="14" t="s">
         <v>421</v>
-      </c>
-      <c r="D200" s="14" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="201" spans="3:4">
       <c r="C201" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="D201" s="14" t="s">
         <v>423</v>
-      </c>
-      <c r="D201" s="14" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="202" spans="3:4">
       <c r="C202" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="D202" s="14" t="s">
         <v>425</v>
-      </c>
-      <c r="D202" s="14" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="203" spans="3:4">
       <c r="C203" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="D203" s="14" t="s">
         <v>427</v>
-      </c>
-      <c r="D203" s="14" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="204" spans="3:4">
       <c r="C204" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="D204" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="D204" s="14" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="205" spans="3:4">
       <c r="C205" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="D205" s="14" t="s">
         <v>431</v>
-      </c>
-      <c r="D205" s="14" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="206" spans="3:4">
       <c r="C206" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="D206" s="14" t="s">
         <v>433</v>
-      </c>
-      <c r="D206" s="14" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="207" spans="3:4">
       <c r="C207" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="D207" s="14" t="s">
         <v>435</v>
-      </c>
-      <c r="D207" s="14" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="208" spans="3:4">
       <c r="C208" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="D208" s="14" t="s">
         <v>437</v>
-      </c>
-      <c r="D208" s="14" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="209" spans="3:4">
       <c r="C209" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="D209" s="14" t="s">
         <v>439</v>
-      </c>
-      <c r="D209" s="14" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="210" spans="3:4">
       <c r="C210" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="D210" s="14" t="s">
         <v>441</v>
-      </c>
-      <c r="D210" s="14" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="211" spans="3:4">
       <c r="C211" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="D211" s="14" t="s">
         <v>443</v>
-      </c>
-      <c r="D211" s="14" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="212" spans="3:4">
       <c r="C212" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="D212" s="14" t="s">
         <v>445</v>
-      </c>
-      <c r="D212" s="14" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="213" spans="3:4">
       <c r="C213" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D213" s="14" t="s">
         <v>447</v>
-      </c>
-      <c r="D213" s="14" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="214" spans="3:4">
       <c r="C214" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="D214" s="14" t="s">
         <v>449</v>
-      </c>
-      <c r="D214" s="14" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="215" spans="3:4">
       <c r="C215" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="D215" s="14" t="s">
         <v>451</v>
-      </c>
-      <c r="D215" s="14" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="216" spans="3:4">
       <c r="C216" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="D216" s="14" t="s">
         <v>453</v>
-      </c>
-      <c r="D216" s="14" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="217" spans="3:4">
       <c r="C217" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="D217" s="14" t="s">
         <v>455</v>
-      </c>
-      <c r="D217" s="14" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="218" spans="3:4">
       <c r="C218" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="D218" s="14" t="s">
         <v>457</v>
-      </c>
-      <c r="D218" s="14" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="219" spans="3:4">
       <c r="C219" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="D219" s="14" t="s">
         <v>459</v>
-      </c>
-      <c r="D219" s="14" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="220" spans="3:4">
       <c r="C220" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="D220" s="14" t="s">
         <v>461</v>
-      </c>
-      <c r="D220" s="14" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="221" spans="3:4">
       <c r="C221" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="D221" s="14" t="s">
         <v>463</v>
-      </c>
-      <c r="D221" s="14" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="222" spans="3:4">
       <c r="C222" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="D222" s="14" t="s">
         <v>465</v>
-      </c>
-      <c r="D222" s="14" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="223" spans="3:4">
       <c r="C223" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="D223" s="14" t="s">
         <v>467</v>
-      </c>
-      <c r="D223" s="14" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="224" spans="3:4">
       <c r="C224" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="D224" s="14" t="s">
         <v>469</v>
-      </c>
-      <c r="D224" s="14" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="225" spans="3:4">
       <c r="C225" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="D225" s="14" t="s">
         <v>471</v>
-      </c>
-      <c r="D225" s="14" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="226" spans="3:4">
       <c r="C226" s="13" t="s">
+        <v>472</v>
+      </c>
+      <c r="D226" s="14" t="s">
         <v>473</v>
-      </c>
-      <c r="D226" s="14" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="227" spans="3:4">
       <c r="C227" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="D227" s="14" t="s">
         <v>475</v>
-      </c>
-      <c r="D227" s="14" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="228" spans="3:4">
       <c r="C228" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="D228" s="14" t="s">
         <v>477</v>
-      </c>
-      <c r="D228" s="14" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="229" spans="3:4">
       <c r="C229" s="13" t="s">
+        <v>478</v>
+      </c>
+      <c r="D229" s="14" t="s">
         <v>479</v>
-      </c>
-      <c r="D229" s="14" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="230" spans="3:4">
       <c r="C230" s="13" t="s">
+        <v>480</v>
+      </c>
+      <c r="D230" s="14" t="s">
         <v>481</v>
-      </c>
-      <c r="D230" s="14" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="231" spans="3:4">
       <c r="C231" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="D231" s="14" t="s">
         <v>483</v>
-      </c>
-      <c r="D231" s="14" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="232" spans="3:4">
       <c r="C232" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="D232" s="14" t="s">
         <v>485</v>
-      </c>
-      <c r="D232" s="14" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="233" spans="3:4">
       <c r="C233" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="D233" s="14" t="s">
         <v>487</v>
-      </c>
-      <c r="D233" s="14" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="234" spans="3:4">
       <c r="C234" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="D234" s="14" t="s">
         <v>489</v>
-      </c>
-      <c r="D234" s="14" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="235" spans="3:4">
       <c r="C235" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="D235" s="14" t="s">
         <v>491</v>
-      </c>
-      <c r="D235" s="14" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="236" spans="3:4">
       <c r="C236" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="D236" s="14" t="s">
         <v>493</v>
-      </c>
-      <c r="D236" s="14" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="237" spans="3:4">
       <c r="C237" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="D237" s="14" t="s">
         <v>495</v>
-      </c>
-      <c r="D237" s="14" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="238" spans="3:4">
       <c r="C238" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="D238" s="14" t="s">
         <v>497</v>
-      </c>
-      <c r="D238" s="14" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="239" spans="3:4">
       <c r="C239" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="D239" s="14" t="s">
         <v>499</v>
-      </c>
-      <c r="D239" s="14" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="240" spans="3:4">
       <c r="C240" s="13" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D240" s="14" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="241" spans="3:4">
       <c r="C241" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="D241" s="14" t="s">
         <v>502</v>
-      </c>
-      <c r="D241" s="14" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="242" spans="3:4">
       <c r="C242" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="D242" s="14" t="s">
         <v>504</v>
-      </c>
-      <c r="D242" s="14" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="243" spans="3:4">
       <c r="C243" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="D243" s="14" t="s">
         <v>506</v>
-      </c>
-      <c r="D243" s="14" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="244" spans="3:4">
       <c r="C244" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="D244" s="14" t="s">
         <v>508</v>
-      </c>
-      <c r="D244" s="14" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="245" spans="3:4">
       <c r="C245" s="13" t="s">
+        <v>509</v>
+      </c>
+      <c r="D245" s="14" t="s">
         <v>510</v>
-      </c>
-      <c r="D245" s="14" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="246" spans="3:4">
       <c r="C246" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="D246" s="14" t="s">
         <v>512</v>
-      </c>
-      <c r="D246" s="14" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="247" spans="3:4">
       <c r="C247" s="13" t="s">
+        <v>513</v>
+      </c>
+      <c r="D247" s="14" t="s">
         <v>514</v>
-      </c>
-      <c r="D247" s="14" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="248" spans="3:4">
       <c r="C248" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="D248" s="14" t="s">
         <v>516</v>
-      </c>
-      <c r="D248" s="14" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="249" spans="3:4">
       <c r="C249" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="D249" s="14" t="s">
         <v>518</v>
-      </c>
-      <c r="D249" s="14" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="250" spans="3:4">
       <c r="C250" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="D250" s="16" t="s">
         <v>520</v>
-      </c>
-      <c r="D250" s="16" t="s">
-        <v>521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IEN-890 | change education column as spreadsheet (#636)
* change education column as spreadsheet

* fix e2e test

* update xlsx file to new column
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunghwan.park/git/ien/apps/web/cypress/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eycanada-my.sharepoint.com/personal/jerry_wang_ca_ey_com/Documents/Documents/projects/jerry/internationally-educated-nurses/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15588D6E-998E-8347-9397-827BAD622748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{15588D6E-998E-8347-9397-827BAD622748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C70F60A-646A-8C4C-A3F5-32B9362E166B}"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="-15680" windowWidth="23820" windowHeight="15680" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20360" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Template - DO NOT EDIT" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Country of Education</t>
-  </si>
-  <si>
     <t>Registration Designation</t>
   </si>
   <si>
@@ -1676,6 +1673,9 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>ISO Code - Education</t>
   </si>
 </sst>
 </file>
@@ -1950,9 +1950,9 @@
     <tableColumn id="9" xr3:uid="{C29B86CB-35D1-4A90-988C-B376D1F11746}" name="State/Province" dataDxfId="5"/>
     <tableColumn id="10" xr3:uid="{51680233-1ACB-4042-AB01-CF531A1CA912}" name="Country"/>
     <tableColumn id="11" xr3:uid="{7CBE1023-D597-4113-A0E3-6BF724D0B2F5}" name="Zip/Postal Code"/>
-    <tableColumn id="14" xr3:uid="{B2EE4131-382E-447B-8582-93712B4E1CE0}" name="Country of Education"/>
+    <tableColumn id="14" xr3:uid="{B2EE4131-382E-447B-8582-93712B4E1CE0}" name="ISO Code - Education"/>
     <tableColumn id="13" xr3:uid="{312FBB00-E05F-4292-8BE8-67886879CB82}" name="ISO Code" dataDxfId="4">
-      <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[Country of Education]],Sheet1!C2:D250,2,0),"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[ISO Code - Education]],Sheet1!C2:D250,2,0),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{A3485428-BB17-4719-9693-9A5D42422885}" name="Date ROS Contract Signed" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{C528BBBE-AF13-4DE4-8CB9-6A5D36322874}" name="NCAS Assessment Complete" dataDxfId="2"/>
@@ -1964,9 +1964,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2004,7 +2004,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2110,7 +2110,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2252,7 +2252,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2262,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:N4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2289,7 +2289,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -2316,22 +2316,22 @@
         <v>12</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>15</v>
+        <v>545</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -2339,19 +2339,19 @@
         <v>112374</v>
       </c>
       <c r="C2" t="s">
+        <v>534</v>
+      </c>
+      <c r="D2" t="s">
+        <v>533</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>535</v>
       </c>
-      <c r="D2" t="s">
-        <v>534</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>536</v>
-      </c>
       <c r="I2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="M2" s="9">
         <v>44562</v>
@@ -2363,7 +2363,7 @@
         <v>13</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2371,19 +2371,19 @@
         <v>111166</v>
       </c>
       <c r="C3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D3" t="s">
+        <v>530</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>532</v>
       </c>
-      <c r="D3" t="s">
-        <v>531</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>533</v>
-      </c>
       <c r="I3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="M3" s="9">
         <v>44593</v>
@@ -2395,7 +2395,7 @@
         <v>13</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -2403,23 +2403,23 @@
         <v>111208</v>
       </c>
       <c r="C4" t="s">
+        <v>537</v>
+      </c>
+      <c r="D4" t="s">
+        <v>536</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>538</v>
       </c>
-      <c r="D4" t="s">
-        <v>537</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>539</v>
-      </c>
       <c r="I4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="N4" s="9"/>
       <c r="O4" s="11" t="s">
         <v>14</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2427,19 +2427,19 @@
         <v>111631</v>
       </c>
       <c r="C5" t="s">
+        <v>541</v>
+      </c>
+      <c r="D5" t="s">
         <v>542</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="17" t="s">
         <v>543</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="I5" t="s">
+        <v>524</v>
+      </c>
+      <c r="K5" t="s">
         <v>544</v>
-      </c>
-      <c r="I5" t="s">
-        <v>525</v>
-      </c>
-      <c r="K5" t="s">
-        <v>545</v>
       </c>
       <c r="N5" s="11" t="s">
         <v>14</v>
@@ -2448,7 +2448,7 @@
         <v>14</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -2456,19 +2456,19 @@
         <v>999999</v>
       </c>
       <c r="C6" t="s">
+        <v>526</v>
+      </c>
+      <c r="D6" t="s">
+        <v>525</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>527</v>
       </c>
-      <c r="D6" t="s">
-        <v>526</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>528</v>
-      </c>
       <c r="I6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="N6" s="11" t="s">
         <v>14</v>
@@ -2477,7 +2477,7 @@
         <v>14</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3163,7 +3163,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -3246,16 +3246,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>522</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3263,13 +3263,13 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3277,2001 +3277,2001 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="C8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="C10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="C11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="C12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="C13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="C14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="C15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="C16" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="3:4">
       <c r="C19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="3:4">
       <c r="C20" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="3:4">
       <c r="C21" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="3:4">
       <c r="C22" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>67</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="3:4">
       <c r="C24" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="3:4">
       <c r="C25" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="3:4">
       <c r="C26" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="27" spans="3:4">
       <c r="C27" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="28" spans="3:4">
       <c r="C28" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>77</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="29" spans="3:4">
       <c r="C29" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="30" spans="3:4">
       <c r="C30" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="31" spans="3:4">
       <c r="C31" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="3:4">
       <c r="C32" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="14" t="s">
         <v>85</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="14" t="s">
         <v>87</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>91</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>101</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="14" t="s">
         <v>107</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>109</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" s="14" t="s">
         <v>123</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55" s="14" t="s">
         <v>131</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D56" s="14" t="s">
         <v>133</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>137</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>139</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D61" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D63" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D64" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" s="14" t="s">
         <v>151</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D67" s="14" t="s">
         <v>155</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D68" s="14" t="s">
         <v>157</v>
-      </c>
-      <c r="D68" s="14" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D69" s="14" t="s">
         <v>159</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D70" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D71" s="14" t="s">
         <v>163</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D72" s="14" t="s">
         <v>165</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D73" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D74" s="14" t="s">
         <v>169</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D75" s="14" t="s">
         <v>171</v>
-      </c>
-      <c r="D75" s="14" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D76" s="14" t="s">
         <v>173</v>
-      </c>
-      <c r="D76" s="14" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D77" s="14" t="s">
         <v>175</v>
-      </c>
-      <c r="D77" s="14" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="D78" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="D78" s="14" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="D79" s="14" t="s">
         <v>179</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D80" s="14" t="s">
         <v>181</v>
-      </c>
-      <c r="D80" s="14" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="81" spans="3:4">
       <c r="C81" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D81" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="82" spans="3:4">
       <c r="C82" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D82" s="14" t="s">
         <v>185</v>
-      </c>
-      <c r="D82" s="14" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="83" spans="3:4">
       <c r="C83" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D83" s="14" t="s">
         <v>187</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="84" spans="3:4">
       <c r="C84" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D84" s="14" t="s">
         <v>189</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="85" spans="3:4">
       <c r="C85" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D85" s="14" t="s">
         <v>191</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="86" spans="3:4">
       <c r="C86" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D86" s="14" t="s">
         <v>193</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="87" spans="3:4">
       <c r="C87" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" s="14" t="s">
         <v>195</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="88" spans="3:4">
       <c r="C88" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D88" s="14" t="s">
         <v>197</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="89" spans="3:4">
       <c r="C89" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D89" s="14" t="s">
         <v>199</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="90" spans="3:4">
       <c r="C90" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D90" s="14" t="s">
         <v>201</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="91" spans="3:4">
       <c r="C91" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D91" s="14" t="s">
         <v>203</v>
-      </c>
-      <c r="D91" s="14" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="92" spans="3:4">
       <c r="C92" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D92" s="14" t="s">
         <v>205</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="93" spans="3:4">
       <c r="C93" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="D93" s="14" t="s">
         <v>207</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="94" spans="3:4">
       <c r="C94" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D94" s="14" t="s">
         <v>209</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="95" spans="3:4">
       <c r="C95" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D95" s="14" t="s">
         <v>211</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="96" spans="3:4">
       <c r="C96" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="D96" s="14" t="s">
         <v>213</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="97" spans="3:4">
       <c r="C97" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D97" s="14" t="s">
         <v>215</v>
-      </c>
-      <c r="D97" s="14" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="98" spans="3:4">
       <c r="C98" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D98" s="14" t="s">
         <v>217</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="99" spans="3:4">
       <c r="C99" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D99" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="D99" s="14" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="100" spans="3:4">
       <c r="C100" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D100" s="14" t="s">
         <v>221</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="101" spans="3:4">
       <c r="C101" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D101" s="14" t="s">
         <v>223</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="102" spans="3:4">
       <c r="C102" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D102" s="14" t="s">
         <v>225</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="103" spans="3:4">
       <c r="C103" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D103" s="14" t="s">
         <v>227</v>
-      </c>
-      <c r="D103" s="14" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="104" spans="3:4">
       <c r="C104" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D104" s="14" t="s">
         <v>229</v>
-      </c>
-      <c r="D104" s="14" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="105" spans="3:4">
       <c r="C105" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D105" s="14" t="s">
         <v>231</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="106" spans="3:4">
       <c r="C106" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D106" s="14" t="s">
         <v>233</v>
-      </c>
-      <c r="D106" s="14" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="107" spans="3:4">
       <c r="C107" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D107" s="14" t="s">
         <v>235</v>
-      </c>
-      <c r="D107" s="14" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="108" spans="3:4">
       <c r="C108" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D108" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="D108" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="109" spans="3:4">
       <c r="C109" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D109" s="14" t="s">
         <v>239</v>
-      </c>
-      <c r="D109" s="14" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="110" spans="3:4">
       <c r="C110" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D110" s="14" t="s">
         <v>241</v>
-      </c>
-      <c r="D110" s="14" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="111" spans="3:4">
       <c r="C111" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D111" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="D111" s="14" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="112" spans="3:4">
       <c r="C112" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D112" s="14" t="s">
         <v>245</v>
-      </c>
-      <c r="D112" s="14" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="113" spans="3:4">
       <c r="C113" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="D113" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="D113" s="14" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="114" spans="3:4">
       <c r="C114" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D114" s="14" t="s">
         <v>249</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="115" spans="3:4">
       <c r="C115" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D115" s="14" t="s">
         <v>251</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="116" spans="3:4">
       <c r="C116" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D116" s="14" t="s">
         <v>253</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="117" spans="3:4">
       <c r="C117" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="D117" s="14" t="s">
         <v>255</v>
-      </c>
-      <c r="D117" s="14" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="118" spans="3:4">
       <c r="C118" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="D118" s="14" t="s">
         <v>257</v>
-      </c>
-      <c r="D118" s="14" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="119" spans="3:4">
       <c r="C119" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="D119" s="14" t="s">
         <v>259</v>
-      </c>
-      <c r="D119" s="14" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="120" spans="3:4">
       <c r="C120" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D120" s="14" t="s">
         <v>261</v>
-      </c>
-      <c r="D120" s="14" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="121" spans="3:4">
       <c r="C121" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D121" s="14" t="s">
         <v>263</v>
-      </c>
-      <c r="D121" s="14" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="122" spans="3:4">
       <c r="C122" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D122" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="D122" s="14" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="123" spans="3:4">
       <c r="C123" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D123" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="D123" s="14" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="124" spans="3:4">
       <c r="C124" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D124" s="14" t="s">
         <v>269</v>
-      </c>
-      <c r="D124" s="14" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="125" spans="3:4">
       <c r="C125" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D125" s="14" t="s">
         <v>271</v>
-      </c>
-      <c r="D125" s="14" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="126" spans="3:4">
       <c r="C126" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D126" s="14" t="s">
         <v>273</v>
-      </c>
-      <c r="D126" s="14" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="127" spans="3:4">
       <c r="C127" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="D127" s="14" t="s">
         <v>275</v>
-      </c>
-      <c r="D127" s="14" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="128" spans="3:4">
       <c r="C128" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="D128" s="14" t="s">
         <v>277</v>
-      </c>
-      <c r="D128" s="14" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="129" spans="3:4">
       <c r="C129" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D129" s="14" t="s">
         <v>279</v>
-      </c>
-      <c r="D129" s="14" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="130" spans="3:4">
       <c r="C130" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="D130" s="14" t="s">
         <v>281</v>
-      </c>
-      <c r="D130" s="14" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="131" spans="3:4">
       <c r="C131" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D131" s="14" t="s">
         <v>283</v>
-      </c>
-      <c r="D131" s="14" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="132" spans="3:4">
       <c r="C132" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D132" s="14" t="s">
         <v>285</v>
-      </c>
-      <c r="D132" s="14" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="133" spans="3:4">
       <c r="C133" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D133" s="14" t="s">
         <v>287</v>
-      </c>
-      <c r="D133" s="14" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="134" spans="3:4">
       <c r="C134" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="D134" s="14" t="s">
         <v>289</v>
-      </c>
-      <c r="D134" s="14" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="135" spans="3:4">
       <c r="C135" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D135" s="14" t="s">
         <v>291</v>
-      </c>
-      <c r="D135" s="14" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="136" spans="3:4">
       <c r="C136" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="D136" s="14" t="s">
         <v>293</v>
-      </c>
-      <c r="D136" s="14" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="137" spans="3:4">
       <c r="C137" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D137" s="14" t="s">
         <v>295</v>
-      </c>
-      <c r="D137" s="14" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="138" spans="3:4">
       <c r="C138" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="D138" s="14" t="s">
         <v>297</v>
-      </c>
-      <c r="D138" s="14" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="139" spans="3:4">
       <c r="C139" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="D139" s="14" t="s">
         <v>299</v>
-      </c>
-      <c r="D139" s="14" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="140" spans="3:4">
       <c r="C140" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D140" s="14" t="s">
         <v>301</v>
-      </c>
-      <c r="D140" s="14" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="141" spans="3:4">
       <c r="C141" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D141" s="14" t="s">
         <v>303</v>
-      </c>
-      <c r="D141" s="14" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="142" spans="3:4">
       <c r="C142" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="D142" s="14" t="s">
         <v>305</v>
-      </c>
-      <c r="D142" s="14" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="143" spans="3:4">
       <c r="C143" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="D143" s="14" t="s">
         <v>307</v>
-      </c>
-      <c r="D143" s="14" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="144" spans="3:4">
       <c r="C144" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="D144" s="14" t="s">
         <v>309</v>
-      </c>
-      <c r="D144" s="14" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="145" spans="3:4">
       <c r="C145" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D145" s="14" t="s">
         <v>311</v>
-      </c>
-      <c r="D145" s="14" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="146" spans="3:4">
       <c r="C146" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="D146" s="14" t="s">
         <v>313</v>
-      </c>
-      <c r="D146" s="14" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="147" spans="3:4">
       <c r="C147" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="D147" s="14" t="s">
         <v>315</v>
-      </c>
-      <c r="D147" s="14" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="148" spans="3:4">
       <c r="C148" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D148" s="14" t="s">
         <v>317</v>
-      </c>
-      <c r="D148" s="14" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="149" spans="3:4">
       <c r="C149" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="D149" s="14" t="s">
         <v>319</v>
-      </c>
-      <c r="D149" s="14" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="150" spans="3:4">
       <c r="C150" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="D150" s="14" t="s">
         <v>321</v>
-      </c>
-      <c r="D150" s="14" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="151" spans="3:4">
       <c r="C151" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="D151" s="14" t="s">
         <v>323</v>
-      </c>
-      <c r="D151" s="14" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="152" spans="3:4">
       <c r="C152" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="D152" s="14" t="s">
         <v>325</v>
-      </c>
-      <c r="D152" s="14" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="153" spans="3:4">
       <c r="C153" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="D153" s="14" t="s">
         <v>327</v>
-      </c>
-      <c r="D153" s="14" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="154" spans="3:4">
       <c r="C154" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="D154" s="14" t="s">
         <v>329</v>
-      </c>
-      <c r="D154" s="14" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="155" spans="3:4">
       <c r="C155" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="D155" s="14" t="s">
         <v>331</v>
-      </c>
-      <c r="D155" s="14" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="156" spans="3:4">
       <c r="C156" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="D156" s="14" t="s">
         <v>333</v>
-      </c>
-      <c r="D156" s="14" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="157" spans="3:4">
       <c r="C157" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="D157" s="14" t="s">
         <v>335</v>
-      </c>
-      <c r="D157" s="14" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="158" spans="3:4">
       <c r="C158" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="D158" s="14" t="s">
         <v>337</v>
-      </c>
-      <c r="D158" s="14" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="159" spans="3:4">
       <c r="C159" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="D159" s="14" t="s">
         <v>339</v>
-      </c>
-      <c r="D159" s="14" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="160" spans="3:4">
       <c r="C160" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="D160" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="D160" s="14" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="161" spans="3:4">
       <c r="C161" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D161" s="14" t="s">
         <v>343</v>
-      </c>
-      <c r="D161" s="14" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="162" spans="3:4">
       <c r="C162" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="D162" s="14" t="s">
         <v>345</v>
-      </c>
-      <c r="D162" s="14" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="163" spans="3:4">
       <c r="C163" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="D163" s="14" t="s">
         <v>347</v>
-      </c>
-      <c r="D163" s="14" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="164" spans="3:4">
       <c r="C164" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="D164" s="14" t="s">
         <v>349</v>
-      </c>
-      <c r="D164" s="14" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="165" spans="3:4">
       <c r="C165" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="D165" s="14" t="s">
         <v>351</v>
-      </c>
-      <c r="D165" s="14" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="166" spans="3:4">
       <c r="C166" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="D166" s="14" t="s">
         <v>353</v>
-      </c>
-      <c r="D166" s="14" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="167" spans="3:4">
       <c r="C167" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="D167" s="14" t="s">
         <v>355</v>
-      </c>
-      <c r="D167" s="14" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="168" spans="3:4">
       <c r="C168" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="D168" s="14" t="s">
         <v>357</v>
-      </c>
-      <c r="D168" s="14" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="169" spans="3:4">
       <c r="C169" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="D169" s="14" t="s">
         <v>359</v>
-      </c>
-      <c r="D169" s="14" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="170" spans="3:4">
       <c r="C170" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="D170" s="14" t="s">
         <v>361</v>
-      </c>
-      <c r="D170" s="14" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="171" spans="3:4">
       <c r="C171" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="D171" s="14" t="s">
         <v>363</v>
-      </c>
-      <c r="D171" s="14" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="172" spans="3:4">
       <c r="C172" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="D172" s="14" t="s">
         <v>365</v>
-      </c>
-      <c r="D172" s="14" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="173" spans="3:4">
       <c r="C173" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="D173" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="D173" s="14" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="174" spans="3:4">
       <c r="C174" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="D174" s="14" t="s">
         <v>369</v>
-      </c>
-      <c r="D174" s="14" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="175" spans="3:4">
       <c r="C175" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="D175" s="14" t="s">
         <v>371</v>
-      </c>
-      <c r="D175" s="14" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="176" spans="3:4">
       <c r="C176" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="D176" s="14" t="s">
         <v>373</v>
-      </c>
-      <c r="D176" s="14" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="177" spans="3:4">
       <c r="C177" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D177" s="14" t="s">
         <v>375</v>
-      </c>
-      <c r="D177" s="14" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="178" spans="3:4">
       <c r="C178" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="D178" s="14" t="s">
         <v>377</v>
-      </c>
-      <c r="D178" s="14" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="179" spans="3:4">
       <c r="C179" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="D179" s="14" t="s">
         <v>379</v>
-      </c>
-      <c r="D179" s="14" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="180" spans="3:4">
       <c r="C180" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="D180" s="14" t="s">
         <v>381</v>
-      </c>
-      <c r="D180" s="14" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="181" spans="3:4">
       <c r="C181" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="D181" s="14" t="s">
         <v>383</v>
-      </c>
-      <c r="D181" s="14" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="182" spans="3:4">
       <c r="C182" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="D182" s="14" t="s">
         <v>385</v>
-      </c>
-      <c r="D182" s="14" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="183" spans="3:4">
       <c r="C183" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D183" s="14" t="s">
         <v>387</v>
-      </c>
-      <c r="D183" s="14" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="184" spans="3:4">
       <c r="C184" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="D184" s="14" t="s">
         <v>389</v>
-      </c>
-      <c r="D184" s="14" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="185" spans="3:4">
       <c r="C185" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="D185" s="14" t="s">
         <v>391</v>
-      </c>
-      <c r="D185" s="14" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="186" spans="3:4">
       <c r="C186" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="D186" s="14" t="s">
         <v>393</v>
-      </c>
-      <c r="D186" s="14" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="187" spans="3:4">
       <c r="C187" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="D187" s="14" t="s">
         <v>395</v>
-      </c>
-      <c r="D187" s="14" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="188" spans="3:4">
       <c r="C188" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="D188" s="14" t="s">
         <v>397</v>
-      </c>
-      <c r="D188" s="14" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="189" spans="3:4">
       <c r="C189" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="D189" s="14" t="s">
         <v>399</v>
-      </c>
-      <c r="D189" s="14" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="190" spans="3:4">
       <c r="C190" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="D190" s="14" t="s">
         <v>401</v>
-      </c>
-      <c r="D190" s="14" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="191" spans="3:4">
       <c r="C191" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="D191" s="14" t="s">
         <v>403</v>
-      </c>
-      <c r="D191" s="14" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="192" spans="3:4">
       <c r="C192" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="D192" s="14" t="s">
         <v>405</v>
-      </c>
-      <c r="D192" s="14" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="193" spans="3:4">
       <c r="C193" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="D193" s="14" t="s">
         <v>407</v>
-      </c>
-      <c r="D193" s="14" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="194" spans="3:4">
       <c r="C194" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="D194" s="14" t="s">
         <v>409</v>
-      </c>
-      <c r="D194" s="14" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="195" spans="3:4">
       <c r="C195" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="D195" s="14" t="s">
         <v>411</v>
-      </c>
-      <c r="D195" s="14" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="196" spans="3:4">
       <c r="C196" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="D196" s="14" t="s">
         <v>413</v>
-      </c>
-      <c r="D196" s="14" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="197" spans="3:4">
       <c r="C197" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="D197" s="14" t="s">
         <v>415</v>
-      </c>
-      <c r="D197" s="14" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="198" spans="3:4">
       <c r="C198" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="D198" s="14" t="s">
         <v>417</v>
-      </c>
-      <c r="D198" s="14" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="199" spans="3:4">
       <c r="C199" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="D199" s="14" t="s">
         <v>419</v>
-      </c>
-      <c r="D199" s="14" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="200" spans="3:4">
       <c r="C200" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="D200" s="14" t="s">
         <v>421</v>
-      </c>
-      <c r="D200" s="14" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="201" spans="3:4">
       <c r="C201" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="D201" s="14" t="s">
         <v>423</v>
-      </c>
-      <c r="D201" s="14" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="202" spans="3:4">
       <c r="C202" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="D202" s="14" t="s">
         <v>425</v>
-      </c>
-      <c r="D202" s="14" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="203" spans="3:4">
       <c r="C203" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="D203" s="14" t="s">
         <v>427</v>
-      </c>
-      <c r="D203" s="14" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="204" spans="3:4">
       <c r="C204" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="D204" s="14" t="s">
         <v>429</v>
-      </c>
-      <c r="D204" s="14" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="205" spans="3:4">
       <c r="C205" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="D205" s="14" t="s">
         <v>431</v>
-      </c>
-      <c r="D205" s="14" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="206" spans="3:4">
       <c r="C206" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="D206" s="14" t="s">
         <v>433</v>
-      </c>
-      <c r="D206" s="14" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="207" spans="3:4">
       <c r="C207" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="D207" s="14" t="s">
         <v>435</v>
-      </c>
-      <c r="D207" s="14" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="208" spans="3:4">
       <c r="C208" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="D208" s="14" t="s">
         <v>437</v>
-      </c>
-      <c r="D208" s="14" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="209" spans="3:4">
       <c r="C209" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="D209" s="14" t="s">
         <v>439</v>
-      </c>
-      <c r="D209" s="14" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="210" spans="3:4">
       <c r="C210" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="D210" s="14" t="s">
         <v>441</v>
-      </c>
-      <c r="D210" s="14" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="211" spans="3:4">
       <c r="C211" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="D211" s="14" t="s">
         <v>443</v>
-      </c>
-      <c r="D211" s="14" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="212" spans="3:4">
       <c r="C212" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="D212" s="14" t="s">
         <v>445</v>
-      </c>
-      <c r="D212" s="14" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="213" spans="3:4">
       <c r="C213" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D213" s="14" t="s">
         <v>447</v>
-      </c>
-      <c r="D213" s="14" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="214" spans="3:4">
       <c r="C214" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="D214" s="14" t="s">
         <v>449</v>
-      </c>
-      <c r="D214" s="14" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="215" spans="3:4">
       <c r="C215" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="D215" s="14" t="s">
         <v>451</v>
-      </c>
-      <c r="D215" s="14" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="216" spans="3:4">
       <c r="C216" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="D216" s="14" t="s">
         <v>453</v>
-      </c>
-      <c r="D216" s="14" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="217" spans="3:4">
       <c r="C217" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="D217" s="14" t="s">
         <v>455</v>
-      </c>
-      <c r="D217" s="14" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="218" spans="3:4">
       <c r="C218" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="D218" s="14" t="s">
         <v>457</v>
-      </c>
-      <c r="D218" s="14" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="219" spans="3:4">
       <c r="C219" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="D219" s="14" t="s">
         <v>459</v>
-      </c>
-      <c r="D219" s="14" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="220" spans="3:4">
       <c r="C220" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="D220" s="14" t="s">
         <v>461</v>
-      </c>
-      <c r="D220" s="14" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="221" spans="3:4">
       <c r="C221" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="D221" s="14" t="s">
         <v>463</v>
-      </c>
-      <c r="D221" s="14" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="222" spans="3:4">
       <c r="C222" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="D222" s="14" t="s">
         <v>465</v>
-      </c>
-      <c r="D222" s="14" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="223" spans="3:4">
       <c r="C223" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="D223" s="14" t="s">
         <v>467</v>
-      </c>
-      <c r="D223" s="14" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="224" spans="3:4">
       <c r="C224" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="D224" s="14" t="s">
         <v>469</v>
-      </c>
-      <c r="D224" s="14" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="225" spans="3:4">
       <c r="C225" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="D225" s="14" t="s">
         <v>471</v>
-      </c>
-      <c r="D225" s="14" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="226" spans="3:4">
       <c r="C226" s="13" t="s">
+        <v>472</v>
+      </c>
+      <c r="D226" s="14" t="s">
         <v>473</v>
-      </c>
-      <c r="D226" s="14" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="227" spans="3:4">
       <c r="C227" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="D227" s="14" t="s">
         <v>475</v>
-      </c>
-      <c r="D227" s="14" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="228" spans="3:4">
       <c r="C228" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="D228" s="14" t="s">
         <v>477</v>
-      </c>
-      <c r="D228" s="14" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="229" spans="3:4">
       <c r="C229" s="13" t="s">
+        <v>478</v>
+      </c>
+      <c r="D229" s="14" t="s">
         <v>479</v>
-      </c>
-      <c r="D229" s="14" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="230" spans="3:4">
       <c r="C230" s="13" t="s">
+        <v>480</v>
+      </c>
+      <c r="D230" s="14" t="s">
         <v>481</v>
-      </c>
-      <c r="D230" s="14" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="231" spans="3:4">
       <c r="C231" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="D231" s="14" t="s">
         <v>483</v>
-      </c>
-      <c r="D231" s="14" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="232" spans="3:4">
       <c r="C232" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="D232" s="14" t="s">
         <v>485</v>
-      </c>
-      <c r="D232" s="14" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="233" spans="3:4">
       <c r="C233" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="D233" s="14" t="s">
         <v>487</v>
-      </c>
-      <c r="D233" s="14" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="234" spans="3:4">
       <c r="C234" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="D234" s="14" t="s">
         <v>489</v>
-      </c>
-      <c r="D234" s="14" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="235" spans="3:4">
       <c r="C235" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="D235" s="14" t="s">
         <v>491</v>
-      </c>
-      <c r="D235" s="14" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="236" spans="3:4">
       <c r="C236" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="D236" s="14" t="s">
         <v>493</v>
-      </c>
-      <c r="D236" s="14" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="237" spans="3:4">
       <c r="C237" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="D237" s="14" t="s">
         <v>495</v>
-      </c>
-      <c r="D237" s="14" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="238" spans="3:4">
       <c r="C238" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="D238" s="14" t="s">
         <v>497</v>
-      </c>
-      <c r="D238" s="14" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="239" spans="3:4">
       <c r="C239" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="D239" s="14" t="s">
         <v>499</v>
-      </c>
-      <c r="D239" s="14" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="240" spans="3:4">
       <c r="C240" s="13" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D240" s="14" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="241" spans="3:4">
       <c r="C241" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="D241" s="14" t="s">
         <v>502</v>
-      </c>
-      <c r="D241" s="14" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="242" spans="3:4">
       <c r="C242" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="D242" s="14" t="s">
         <v>504</v>
-      </c>
-      <c r="D242" s="14" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="243" spans="3:4">
       <c r="C243" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="D243" s="14" t="s">
         <v>506</v>
-      </c>
-      <c r="D243" s="14" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="244" spans="3:4">
       <c r="C244" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="D244" s="14" t="s">
         <v>508</v>
-      </c>
-      <c r="D244" s="14" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="245" spans="3:4">
       <c r="C245" s="13" t="s">
+        <v>509</v>
+      </c>
+      <c r="D245" s="14" t="s">
         <v>510</v>
-      </c>
-      <c r="D245" s="14" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="246" spans="3:4">
       <c r="C246" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="D246" s="14" t="s">
         <v>512</v>
-      </c>
-      <c r="D246" s="14" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="247" spans="3:4">
       <c r="C247" s="13" t="s">
+        <v>513</v>
+      </c>
+      <c r="D247" s="14" t="s">
         <v>514</v>
-      </c>
-      <c r="D247" s="14" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="248" spans="3:4">
       <c r="C248" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="D248" s="14" t="s">
         <v>516</v>
-      </c>
-      <c r="D248" s="14" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="249" spans="3:4">
       <c r="C249" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="D249" s="14" t="s">
         <v>518</v>
-      </c>
-      <c r="D249" s="14" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="250" spans="3:4">
       <c r="C250" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="D250" s="16" t="s">
         <v>520</v>
-      </c>
-      <c r="D250" s="16" t="s">
-        <v>521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed test data and addressed sonar cloud warnings
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/_Never Backup/internationally-educated-nurses/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1586A144-491C-0440-A524-2AF4AD2FEF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A08BDBF-331F-644C-893F-DAAB2F2F1EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="3760" windowWidth="35840" windowHeight="19920" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
+    <workbookView xWindow="-800" yWindow="-20640" windowWidth="38400" windowHeight="20260" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Template - DO NOT EDIT" sheetId="1" r:id="rId1"/>
@@ -1603,9 +1603,6 @@
     <t>jm</t>
   </si>
   <si>
-    <t>ng</t>
-  </si>
-  <si>
     <t>Paris</t>
   </si>
   <si>
@@ -1679,6 +1676,9 @@
   </si>
   <si>
     <t>BCCNM Provisional License RN</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -2334,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:S643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2362,52 +2362,52 @@
         <v>4</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>535</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>536</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>537</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>538</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>539</v>
-      </c>
       <c r="H1" s="17" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="15" t="s">
+        <v>539</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>540</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>541</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="13" t="s">
         <v>542</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>543</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>544</v>
       </c>
       <c r="O1" s="13" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>545</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>546</v>
       </c>
       <c r="R1" s="13" t="s">
         <v>515</v>
@@ -2421,13 +2421,13 @@
         <v>112374</v>
       </c>
       <c r="C2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>526</v>
-      </c>
-      <c r="D2" t="s">
-        <v>525</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>527</v>
       </c>
       <c r="H2" t="s">
         <v>520</v>
@@ -2450,13 +2450,13 @@
         <v>111166</v>
       </c>
       <c r="C3" t="s">
+        <v>522</v>
+      </c>
+      <c r="D3" t="s">
+        <v>521</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>523</v>
-      </c>
-      <c r="D3" t="s">
-        <v>522</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>524</v>
       </c>
       <c r="H3" t="s">
         <v>520</v>
@@ -2479,16 +2479,16 @@
         <v>111208</v>
       </c>
       <c r="C4" t="s">
+        <v>528</v>
+      </c>
+      <c r="D4" t="s">
+        <v>527</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>529</v>
       </c>
-      <c r="D4" t="s">
-        <v>528</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>530</v>
-      </c>
       <c r="H4" t="s">
-        <v>521</v>
+        <v>546</v>
       </c>
       <c r="I4" s="5"/>
       <c r="N4" s="5"/>
@@ -2503,13 +2503,13 @@
         <v>111631</v>
       </c>
       <c r="C5" t="s">
+        <v>530</v>
+      </c>
+      <c r="D5" t="s">
         <v>531</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="12" t="s">
         <v>532</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>533</v>
       </c>
       <c r="H5" t="s">
         <v>516</v>

</xml_diff>

<commit_message>
Updating columns on test spreadsheet
</commit_message>
<xml_diff>
--- a/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
+++ b/apps/web/cypress/fixtures/bccnm-ncas-creates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/_Never Backup/internationally-educated-nurses/apps/web/cypress/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA84D0F-22FC-2849-A9BA-001B2BF62F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50461CE-18F8-3A43-8282-40A529DCE2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="860" windowWidth="35840" windowHeight="19920" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19920" xr2:uid="{D4D11464-A1E4-4602-A7F2-C977BA426C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Template - DO NOT EDIT" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="545">
   <si>
     <t>Date ROS Contract Signed</t>
   </si>
@@ -1666,19 +1666,13 @@
     <t>BCCNM Decision Date</t>
   </si>
   <si>
-    <t>BCCNM Full License LPN</t>
-  </si>
-  <si>
-    <t>BCCNM Full License RN</t>
-  </si>
-  <si>
-    <t>BCCNM Provisional License LPN</t>
-  </si>
-  <si>
-    <t>BCCNM Provisional License RN</t>
-  </si>
-  <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>BCCNM Full Licence RPN</t>
+  </si>
+  <si>
+    <t>BCCNM Provisional Licence RPN</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1682,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -1726,6 +1720,12 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="BC Sans"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1918,7 +1918,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1954,6 +1954,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2023,12 +2026,12 @@
     <tableColumn id="13" xr3:uid="{312FBB00-E05F-4292-8BE8-67886879CB82}" name="BCCNM Decision Date" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table1[[#This Row],[Date BCCNM Application Complete]],Sheet1!C2:D250,2,0),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A3485428-BB17-4719-9693-9A5D42422885}" name="BCCNM Full License LPN" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{C528BBBE-AF13-4DE4-8CB9-6A5D36322874}" name="BCCNM Full License RN" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{FC5EB113-2259-4AAD-B918-D66D8CDC1B70}" name="BCCNM Full License RPN" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{2EEE535B-18BF-4006-8377-F5D12DDCB956}" name="BCCNM Provisional License LPN" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{DEAEBA83-5933-5D41-BE8E-75D5B0FFF967}" name="BCCNM Provisional License RN" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{4C24EF1B-31E4-3B43-8049-AC92376845CE}" name="BCCNM Provisional License RPN" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{A3485428-BB17-4719-9693-9A5D42422885}" name="BCCNM Full Licence LPN" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{C528BBBE-AF13-4DE4-8CB9-6A5D36322874}" name="BCCNM Full Licence RN" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{FC5EB113-2259-4AAD-B918-D66D8CDC1B70}" name="BCCNM Full Licence RPN" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{2EEE535B-18BF-4006-8377-F5D12DDCB956}" name="BCCNM Provisional Licence LPN" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{DEAEBA83-5933-5D41-BE8E-75D5B0FFF967}" name="BCCNM Provisional Licence RN" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{4C24EF1B-31E4-3B43-8049-AC92376845CE}" name="BCCNM Provisional Licence RPN" dataDxfId="1"/>
     <tableColumn id="19" xr3:uid="{1F506AB8-A1A2-DD42-8CC0-4DDAF2FED40D}" name="Registration Designation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2334,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54943090-89AD-474D-AA31-B1A3EE9F8526}">
   <dimension ref="A1:S643"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12"/>
@@ -2394,25 +2397,25 @@
       <c r="L1" s="18" t="s">
         <v>541</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>542</v>
-      </c>
-      <c r="N1" s="13" t="s">
+      <c r="M1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="19" t="s">
         <v>543</v>
       </c>
-      <c r="O1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>544</v>
       </c>
-      <c r="Q1" s="13" t="s">
-        <v>545</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>515</v>
-      </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="19" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2510,7 +2513,7 @@
         <v>532</v>
       </c>
       <c r="H5" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="I5" s="5"/>
       <c r="Q5" s="6"/>

</xml_diff>